<commit_message>
added heart rate, median and heatmap
</commit_message>
<xml_diff>
--- a/Algorithm_tester/data_autosave/real_overall.xlsx
+++ b/Algorithm_tester/data_autosave/real_overall.xlsx
@@ -503,7 +503,7 @@
         <v>0</v>
       </c>
       <c r="E2" t="n">
-        <v>78.09734344482422</v>
+        <v>92.09895133972168</v>
       </c>
       <c r="F2" t="n">
         <v>0</v>
@@ -518,19 +518,19 @@
         <v>0.05</v>
       </c>
       <c r="C3" t="n">
-        <v>0.5796277997364954</v>
+        <v>0</v>
       </c>
       <c r="D3" t="n">
         <v>0</v>
       </c>
       <c r="E3" t="n">
-        <v>91.75467491149902</v>
+        <v>166.1584377288818</v>
       </c>
       <c r="F3" t="n">
-        <v>0.8461538461538461</v>
+        <v>0</v>
       </c>
       <c r="G3" t="n">
-        <v>0.4466185410334347</v>
+        <v>0</v>
       </c>
     </row>
     <row r="4">
@@ -539,19 +539,19 @@
         <v>0.25</v>
       </c>
       <c r="C4" t="n">
-        <v>0.9705882352941176</v>
+        <v>0.4267857142857143</v>
       </c>
       <c r="D4" t="n">
         <v>0</v>
       </c>
       <c r="E4" t="n">
-        <v>109.2272996902466</v>
+        <v>188.88258934021</v>
       </c>
       <c r="F4" t="n">
-        <v>0.9722222222222222</v>
+        <v>0.9714285714285714</v>
       </c>
       <c r="G4" t="n">
-        <v>0.9722222222222222</v>
+        <v>0.2862997658079625</v>
       </c>
     </row>
     <row r="5">
@@ -560,19 +560,19 @@
         <v>0.5</v>
       </c>
       <c r="C5" t="n">
-        <v>0.987012987012987</v>
+        <v>0.9411764705882353</v>
       </c>
       <c r="D5" t="n">
         <v>0</v>
       </c>
       <c r="E5" t="n">
-        <v>176.9394874572754</v>
+        <v>249.0637302398682</v>
       </c>
       <c r="F5" t="n">
         <v>1</v>
       </c>
       <c r="G5" t="n">
-        <v>1</v>
+        <v>0.9375</v>
       </c>
     </row>
     <row r="6">
@@ -581,13 +581,13 @@
         <v>0.75</v>
       </c>
       <c r="C6" t="n">
-        <v>1</v>
+        <v>0.9866666666666667</v>
       </c>
       <c r="D6" t="n">
         <v>0</v>
       </c>
       <c r="E6" t="n">
-        <v>252.2982358932495</v>
+        <v>295.1279878616333</v>
       </c>
       <c r="F6" t="n">
         <v>1</v>
@@ -608,7 +608,7 @@
         <v>0</v>
       </c>
       <c r="E7" t="n">
-        <v>322.3831653594971</v>
+        <v>401.4069318771362</v>
       </c>
       <c r="F7" t="n">
         <v>1</v>
@@ -629,7 +629,7 @@
         <v>0</v>
       </c>
       <c r="E8" t="n">
-        <v>880.8329105377197</v>
+        <v>625.4055500030518</v>
       </c>
       <c r="F8" t="n">
         <v>1</v>
@@ -669,19 +669,19 @@
         <v>0.05</v>
       </c>
       <c r="C10" t="n">
-        <v>0.3555555555555556</v>
+        <v>0</v>
       </c>
       <c r="D10" t="n">
         <v>0</v>
       </c>
       <c r="E10" t="n">
-        <v>36.74221038818359</v>
+        <v>0</v>
       </c>
       <c r="F10" t="n">
-        <v>0.2222222222222222</v>
+        <v>0</v>
       </c>
       <c r="G10" t="n">
-        <v>0.8604651162790697</v>
+        <v>0</v>
       </c>
     </row>
     <row r="11">
@@ -690,19 +690,19 @@
         <v>0.25</v>
       </c>
       <c r="C11" t="n">
-        <v>0.9449201105642824</v>
+        <v>0</v>
       </c>
       <c r="D11" t="n">
         <v>0</v>
       </c>
       <c r="E11" t="n">
-        <v>44.44420337677002</v>
+        <v>64.78762626647949</v>
       </c>
       <c r="F11" t="n">
-        <v>0.9038461538461539</v>
+        <v>0</v>
       </c>
       <c r="G11" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="12">
@@ -711,16 +711,16 @@
         <v>0.5</v>
       </c>
       <c r="C12" t="n">
-        <v>0.9803921568627451</v>
+        <v>0.7951807228915663</v>
       </c>
       <c r="D12" t="n">
         <v>0</v>
       </c>
       <c r="E12" t="n">
-        <v>70.8918571472168</v>
+        <v>86.65943145751953</v>
       </c>
       <c r="F12" t="n">
-        <v>0.9642857142857143</v>
+        <v>0.7586206896551724</v>
       </c>
       <c r="G12" t="n">
         <v>1</v>
@@ -732,16 +732,16 @@
         <v>0.75</v>
       </c>
       <c r="C13" t="n">
-        <v>0.9882352941176471</v>
+        <v>0.9830508474576272</v>
       </c>
       <c r="D13" t="n">
         <v>0</v>
       </c>
       <c r="E13" t="n">
-        <v>101.0836362838745</v>
+        <v>101.6875505447388</v>
       </c>
       <c r="F13" t="n">
-        <v>0.9777777777777777</v>
+        <v>0.9701426024955437</v>
       </c>
       <c r="G13" t="n">
         <v>1</v>
@@ -753,16 +753,16 @@
         <v>0.95</v>
       </c>
       <c r="C14" t="n">
-        <v>1</v>
+        <v>0.9882352941176471</v>
       </c>
       <c r="D14" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E14" t="n">
-        <v>133.1466436386108</v>
+        <v>138.3724927902221</v>
       </c>
       <c r="F14" t="n">
-        <v>1</v>
+        <v>0.9782608695652174</v>
       </c>
       <c r="G14" t="n">
         <v>1</v>
@@ -780,7 +780,7 @@
         <v>1</v>
       </c>
       <c r="E15" t="n">
-        <v>34310.37449836731</v>
+        <v>215.8746719360352</v>
       </c>
       <c r="F15" t="n">
         <v>1</v>
@@ -820,19 +820,19 @@
         <v>0.05</v>
       </c>
       <c r="C17" t="n">
-        <v>0.4954128440366973</v>
+        <v>0.2888888888888889</v>
       </c>
       <c r="D17" t="n">
         <v>0</v>
       </c>
       <c r="E17" t="n">
-        <v>0</v>
+        <v>4.849863052368164</v>
       </c>
       <c r="F17" t="n">
-        <v>1</v>
+        <v>0.9597551020408163</v>
       </c>
       <c r="G17" t="n">
-        <v>0.3292682926829268</v>
+        <v>0.1688311688311688</v>
       </c>
     </row>
     <row r="18">
@@ -841,19 +841,19 @@
         <v>0.25</v>
       </c>
       <c r="C18" t="n">
-        <v>0.5739130434782609</v>
+        <v>0.5102040816326531</v>
       </c>
       <c r="D18" t="n">
         <v>0</v>
       </c>
       <c r="E18" t="n">
-        <v>4.315376281738281</v>
+        <v>6.972312927246094</v>
       </c>
       <c r="F18" t="n">
         <v>1</v>
       </c>
       <c r="G18" t="n">
-        <v>0.4024390243902439</v>
+        <v>0.3443533697632059</v>
       </c>
     </row>
     <row r="19">
@@ -862,19 +862,19 @@
         <v>0.5</v>
       </c>
       <c r="C19" t="n">
-        <v>0.64</v>
+        <v>0.5909090909090909</v>
       </c>
       <c r="D19" t="n">
         <v>0</v>
       </c>
       <c r="E19" t="n">
-        <v>5.98454475402832</v>
+        <v>10.42509078979492</v>
       </c>
       <c r="F19" t="n">
         <v>1</v>
       </c>
       <c r="G19" t="n">
-        <v>0.4712643678160919</v>
+        <v>0.4197530864197531</v>
       </c>
     </row>
     <row r="20">
@@ -883,19 +883,19 @@
         <v>0.75</v>
       </c>
       <c r="C20" t="n">
-        <v>0.7</v>
+        <v>0.6610869869729654</v>
       </c>
       <c r="D20" t="n">
         <v>0</v>
       </c>
       <c r="E20" t="n">
-        <v>9.996771812438965</v>
+        <v>18.05734634399414</v>
       </c>
       <c r="F20" t="n">
         <v>1</v>
       </c>
       <c r="G20" t="n">
-        <v>0.5394736842105263</v>
+        <v>0.4941045914828686</v>
       </c>
     </row>
     <row r="21">
@@ -904,19 +904,19 @@
         <v>0.95</v>
       </c>
       <c r="C21" t="n">
-        <v>0.8201438848920863</v>
+        <v>0.8</v>
       </c>
       <c r="D21" t="n">
         <v>0</v>
       </c>
       <c r="E21" t="n">
-        <v>32.76991844177246</v>
+        <v>89.62256908416747</v>
       </c>
       <c r="F21" t="n">
         <v>1</v>
       </c>
       <c r="G21" t="n">
-        <v>0.6987951807228916</v>
+        <v>0.6678861788617885</v>
       </c>
     </row>
     <row r="22">
@@ -925,19 +925,19 @@
         <v>1</v>
       </c>
       <c r="C22" t="n">
-        <v>1</v>
+        <v>0.9642857142857143</v>
       </c>
       <c r="D22" t="n">
         <v>1</v>
       </c>
       <c r="E22" t="n">
-        <v>267.0910358428955</v>
+        <v>280.9844017028809</v>
       </c>
       <c r="F22" t="n">
         <v>1</v>
       </c>
       <c r="G22" t="n">
-        <v>1</v>
+        <v>0.9310344827586207</v>
       </c>
     </row>
     <row r="23">
@@ -956,7 +956,7 @@
         <v>0</v>
       </c>
       <c r="E23" t="n">
-        <v>31.2812328338623</v>
+        <v>51.86057090759277</v>
       </c>
       <c r="F23" t="n">
         <v>0</v>
@@ -971,19 +971,19 @@
         <v>0.05</v>
       </c>
       <c r="C24" t="n">
-        <v>0.8481554677206851</v>
+        <v>0.3709914320685435</v>
       </c>
       <c r="D24" t="n">
         <v>0</v>
       </c>
       <c r="E24" t="n">
-        <v>49.90649223327637</v>
+        <v>91.00511074066162</v>
       </c>
       <c r="F24" t="n">
-        <v>0.7878787878787878</v>
+        <v>0.6506393861892583</v>
       </c>
       <c r="G24" t="n">
-        <v>0.9622641509433962</v>
+        <v>0.2484693877551021</v>
       </c>
     </row>
     <row r="25">
@@ -992,19 +992,19 @@
         <v>0.25</v>
       </c>
       <c r="C25" t="n">
-        <v>0.9811320754716981</v>
+        <v>0.8155706727135299</v>
       </c>
       <c r="D25" t="n">
         <v>0</v>
       </c>
       <c r="E25" t="n">
-        <v>58.84182453155518</v>
+        <v>118.0760860443115</v>
       </c>
       <c r="F25" t="n">
-        <v>0.967741935483871</v>
+        <v>0.9603921568627451</v>
       </c>
       <c r="G25" t="n">
-        <v>1</v>
+        <v>0.7565656565656566</v>
       </c>
     </row>
     <row r="26">
@@ -1013,16 +1013,16 @@
         <v>0.5</v>
       </c>
       <c r="C26" t="n">
-        <v>0.9890109890109891</v>
+        <v>0.9662921348314607</v>
       </c>
       <c r="D26" t="n">
         <v>0</v>
       </c>
       <c r="E26" t="n">
-        <v>95.95060348510742</v>
+        <v>141.803503036499</v>
       </c>
       <c r="F26" t="n">
-        <v>0.9807692307692307</v>
+        <v>1</v>
       </c>
       <c r="G26" t="n">
         <v>1</v>
@@ -1040,7 +1040,7 @@
         <v>0</v>
       </c>
       <c r="E27" t="n">
-        <v>135.0950002670288</v>
+        <v>172.5533008575439</v>
       </c>
       <c r="F27" t="n">
         <v>1</v>
@@ -1061,7 +1061,7 @@
         <v>0</v>
       </c>
       <c r="E28" t="n">
-        <v>173.3695268630981</v>
+        <v>256.2325239181518</v>
       </c>
       <c r="F28" t="n">
         <v>1</v>
@@ -1082,7 +1082,7 @@
         <v>0</v>
       </c>
       <c r="E29" t="n">
-        <v>8048.917531967163</v>
+        <v>434.6280097961426</v>
       </c>
       <c r="F29" t="n">
         <v>1</v>
@@ -1107,7 +1107,7 @@
         <v>0</v>
       </c>
       <c r="E30" t="n">
-        <v>0</v>
+        <v>7.108211517333984</v>
       </c>
       <c r="F30" t="n">
         <v>0</v>
@@ -1122,19 +1122,19 @@
         <v>0.05</v>
       </c>
       <c r="C31" t="n">
-        <v>0.810126582278481</v>
+        <v>0</v>
       </c>
       <c r="D31" t="n">
         <v>0</v>
       </c>
       <c r="E31" t="n">
-        <v>4.057407379150391</v>
+        <v>9.895062446594238</v>
       </c>
       <c r="F31" t="n">
-        <v>0.8604651162790697</v>
+        <v>0</v>
       </c>
       <c r="G31" t="n">
-        <v>0.7951631701631701</v>
+        <v>0</v>
       </c>
     </row>
     <row r="32">
@@ -1143,19 +1143,19 @@
         <v>0.25</v>
       </c>
       <c r="C32" t="n">
-        <v>0.967741935483871</v>
+        <v>0.3385416666666666</v>
       </c>
       <c r="D32" t="n">
         <v>0</v>
       </c>
       <c r="E32" t="n">
-        <v>8.975505828857422</v>
+        <v>12.96460628509521</v>
       </c>
       <c r="F32" t="n">
-        <v>0.975609756097561</v>
+        <v>0.7336719883889695</v>
       </c>
       <c r="G32" t="n">
-        <v>0.9705882352941176</v>
+        <v>0.244047619047619</v>
       </c>
     </row>
     <row r="33">
@@ -1164,19 +1164,19 @@
         <v>0.5</v>
       </c>
       <c r="C33" t="n">
-        <v>0.9866666666666667</v>
+        <v>0.9473684210526315</v>
       </c>
       <c r="D33" t="n">
         <v>0</v>
       </c>
       <c r="E33" t="n">
-        <v>12.96281814575195</v>
+        <v>18.0671215057373</v>
       </c>
       <c r="F33" t="n">
         <v>1</v>
       </c>
       <c r="G33" t="n">
-        <v>1</v>
+        <v>0.9090909090909091</v>
       </c>
     </row>
     <row r="34">
@@ -1185,19 +1185,19 @@
         <v>0.75</v>
       </c>
       <c r="C34" t="n">
-        <v>1</v>
+        <v>0.9863013698630136</v>
       </c>
       <c r="D34" t="n">
         <v>0</v>
       </c>
       <c r="E34" t="n">
-        <v>19.97542381286621</v>
+        <v>23.93579483032227</v>
       </c>
       <c r="F34" t="n">
         <v>1</v>
       </c>
       <c r="G34" t="n">
-        <v>1</v>
+        <v>0.9761904761904762</v>
       </c>
     </row>
     <row r="35">
@@ -1212,7 +1212,7 @@
         <v>0</v>
       </c>
       <c r="E35" t="n">
-        <v>30.50720691680908</v>
+        <v>34.50999259948729</v>
       </c>
       <c r="F35" t="n">
         <v>1</v>
@@ -1233,7 +1233,7 @@
         <v>0</v>
       </c>
       <c r="E36" t="n">
-        <v>98.3426570892334</v>
+        <v>83.41193199157715</v>
       </c>
       <c r="F36" t="n">
         <v>1</v>
@@ -1273,19 +1273,19 @@
         <v>0.05</v>
       </c>
       <c r="C38" t="n">
-        <v>0.5111111111111111</v>
+        <v>0</v>
       </c>
       <c r="D38" t="n">
         <v>0</v>
       </c>
       <c r="E38" t="n">
-        <v>1.037001609802246</v>
+        <v>9.525275230407715</v>
       </c>
       <c r="F38" t="n">
-        <v>0.34375</v>
+        <v>0</v>
       </c>
       <c r="G38" t="n">
-        <v>0.9743589743589743</v>
+        <v>0</v>
       </c>
     </row>
     <row r="39">
@@ -1294,19 +1294,19 @@
         <v>0.25</v>
       </c>
       <c r="C39" t="n">
-        <v>0.9090909090909091</v>
+        <v>0.6402157164869029</v>
       </c>
       <c r="D39" t="n">
         <v>0</v>
       </c>
       <c r="E39" t="n">
-        <v>9.923577308654785</v>
+        <v>12.64822483062744</v>
       </c>
       <c r="F39" t="n">
-        <v>0.8333333333333334</v>
+        <v>0.6561913696060038</v>
       </c>
       <c r="G39" t="n">
-        <v>1</v>
+        <v>0.7609523809523809</v>
       </c>
     </row>
     <row r="40">
@@ -1315,16 +1315,16 @@
         <v>0.5</v>
       </c>
       <c r="C40" t="n">
-        <v>1</v>
+        <v>0.9152542372881356</v>
       </c>
       <c r="D40" t="n">
         <v>0</v>
       </c>
       <c r="E40" t="n">
-        <v>11.97361946105957</v>
+        <v>15.9294605255127</v>
       </c>
       <c r="F40" t="n">
-        <v>1</v>
+        <v>0.9705882352941176</v>
       </c>
       <c r="G40" t="n">
         <v>1</v>
@@ -1342,7 +1342,7 @@
         <v>0</v>
       </c>
       <c r="E41" t="n">
-        <v>15.94352722167969</v>
+        <v>18.31746101379395</v>
       </c>
       <c r="F41" t="n">
         <v>1</v>
@@ -1363,7 +1363,7 @@
         <v>0</v>
       </c>
       <c r="E42" t="n">
-        <v>24.91283416748047</v>
+        <v>23.61953258514402</v>
       </c>
       <c r="F42" t="n">
         <v>1</v>
@@ -1384,7 +1384,7 @@
         <v>1</v>
       </c>
       <c r="E43" t="n">
-        <v>4190.004587173462</v>
+        <v>744.5070743560791</v>
       </c>
       <c r="F43" t="n">
         <v>1</v>
@@ -1424,19 +1424,19 @@
         <v>0.05</v>
       </c>
       <c r="C45" t="n">
-        <v>0.8461538461538461</v>
+        <v>0</v>
       </c>
       <c r="D45" t="n">
         <v>0</v>
       </c>
       <c r="E45" t="n">
-        <v>0</v>
+        <v>0.7397174835205103</v>
       </c>
       <c r="F45" t="n">
-        <v>0.7916666666666666</v>
+        <v>0</v>
       </c>
       <c r="G45" t="n">
-        <v>0.9393939393939394</v>
+        <v>0</v>
       </c>
     </row>
     <row r="46">
@@ -1445,19 +1445,19 @@
         <v>0.25</v>
       </c>
       <c r="C46" t="n">
-        <v>0.9818181818181818</v>
+        <v>0.2253968253968254</v>
       </c>
       <c r="D46" t="n">
         <v>0</v>
       </c>
       <c r="E46" t="n">
-        <v>2.062201499938965</v>
+        <v>1.999139785766602</v>
       </c>
       <c r="F46" t="n">
-        <v>0.9705882352941176</v>
+        <v>0.3452380952380952</v>
       </c>
       <c r="G46" t="n">
-        <v>1</v>
+        <v>0.1726708074534161</v>
       </c>
     </row>
     <row r="47">
@@ -1466,19 +1466,19 @@
         <v>0.5</v>
       </c>
       <c r="C47" t="n">
-        <v>0.9885057471264368</v>
+        <v>0.9538461538461539</v>
       </c>
       <c r="D47" t="n">
         <v>0</v>
       </c>
       <c r="E47" t="n">
-        <v>2.992630004882812</v>
+        <v>2.991437911987305</v>
       </c>
       <c r="F47" t="n">
-        <v>0.9814814814814815</v>
+        <v>0.9795918367346939</v>
       </c>
       <c r="G47" t="n">
-        <v>1</v>
+        <v>0.9444444444444444</v>
       </c>
     </row>
     <row r="48">
@@ -1487,13 +1487,13 @@
         <v>0.75</v>
       </c>
       <c r="C48" t="n">
-        <v>1</v>
+        <v>0.9890109890109891</v>
       </c>
       <c r="D48" t="n">
         <v>0</v>
       </c>
       <c r="E48" t="n">
-        <v>3.977298736572266</v>
+        <v>2.994894981384277</v>
       </c>
       <c r="F48" t="n">
         <v>1</v>
@@ -1514,7 +1514,7 @@
         <v>0</v>
       </c>
       <c r="E49" t="n">
-        <v>6.038784980773926</v>
+        <v>4.003477096557615</v>
       </c>
       <c r="F49" t="n">
         <v>1</v>
@@ -1535,7 +1535,7 @@
         <v>0</v>
       </c>
       <c r="E50" t="n">
-        <v>135.3557109832764</v>
+        <v>6.981372833251953</v>
       </c>
       <c r="F50" t="n">
         <v>1</v>
@@ -1581,7 +1581,7 @@
         <v>0</v>
       </c>
       <c r="E52" t="n">
-        <v>0</v>
+        <v>2.987957000732422</v>
       </c>
       <c r="F52" t="n">
         <v>0</v>
@@ -1596,19 +1596,19 @@
         <v>0.25</v>
       </c>
       <c r="C53" t="n">
-        <v>0.38379705400982</v>
+        <v>0</v>
       </c>
       <c r="D53" t="n">
         <v>0</v>
       </c>
       <c r="E53" t="n">
-        <v>3.988027572631836</v>
+        <v>3.989219665527344</v>
       </c>
       <c r="F53" t="n">
-        <v>0.2391304347826087</v>
+        <v>0</v>
       </c>
       <c r="G53" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="54">
@@ -1617,19 +1617,19 @@
         <v>0.5</v>
       </c>
       <c r="C54" t="n">
-        <v>0.946236559139785</v>
+        <v>0.7169811320754716</v>
       </c>
       <c r="D54" t="n">
         <v>0</v>
       </c>
       <c r="E54" t="n">
-        <v>4.98652458190918</v>
+        <v>4.986286163330078</v>
       </c>
       <c r="F54" t="n">
-        <v>0.9130434782608695</v>
+        <v>0.625</v>
       </c>
       <c r="G54" t="n">
-        <v>1</v>
+        <v>0.9629629629629629</v>
       </c>
     </row>
     <row r="55">
@@ -1638,13 +1638,13 @@
         <v>0.75</v>
       </c>
       <c r="C55" t="n">
-        <v>1</v>
+        <v>0.9898989898989899</v>
       </c>
       <c r="D55" t="n">
         <v>0</v>
       </c>
       <c r="E55" t="n">
-        <v>6.012201309204102</v>
+        <v>5.983471870422363</v>
       </c>
       <c r="F55" t="n">
         <v>1</v>
@@ -1665,7 +1665,7 @@
         <v>0</v>
       </c>
       <c r="E56" t="n">
-        <v>16.15941524505615</v>
+        <v>7.53355026245117</v>
       </c>
       <c r="F56" t="n">
         <v>1</v>
@@ -1686,7 +1686,7 @@
         <v>0</v>
       </c>
       <c r="E57" t="n">
-        <v>195.0221061706543</v>
+        <v>51.86605453491211</v>
       </c>
       <c r="F57" t="n">
         <v>1</v>
@@ -1711,7 +1711,7 @@
         <v>0</v>
       </c>
       <c r="E58" t="n">
-        <v>0</v>
+        <v>10.0092887878418</v>
       </c>
       <c r="F58" t="n">
         <v>0</v>
@@ -1726,19 +1726,19 @@
         <v>0.05</v>
       </c>
       <c r="C59" t="n">
-        <v>0.8076923076923077</v>
+        <v>0.3720930232558139</v>
       </c>
       <c r="D59" t="n">
         <v>0</v>
       </c>
       <c r="E59" t="n">
-        <v>8.979320526123047</v>
+        <v>17.6771879196167</v>
       </c>
       <c r="F59" t="n">
-        <v>0.725</v>
+        <v>0.3694633408919123</v>
       </c>
       <c r="G59" t="n">
-        <v>0.9696969696969697</v>
+        <v>0.3085457271364318</v>
       </c>
     </row>
     <row r="60">
@@ -1747,19 +1747,19 @@
         <v>0.25</v>
       </c>
       <c r="C60" t="n">
-        <v>0.9696969696969697</v>
+        <v>0.7580487804878049</v>
       </c>
       <c r="D60" t="n">
         <v>0</v>
       </c>
       <c r="E60" t="n">
-        <v>10.98835468292236</v>
+        <v>24.69062805175781</v>
       </c>
       <c r="F60" t="n">
-        <v>0.9433962264150944</v>
+        <v>0.8055555555555556</v>
       </c>
       <c r="G60" t="n">
-        <v>1</v>
+        <v>0.7752525252525253</v>
       </c>
     </row>
     <row r="61">
@@ -1768,16 +1768,16 @@
         <v>0.5</v>
       </c>
       <c r="C61" t="n">
-        <v>0.9830508474576272</v>
+        <v>0.9523809523809523</v>
       </c>
       <c r="D61" t="n">
         <v>0</v>
       </c>
       <c r="E61" t="n">
-        <v>21.46005630493164</v>
+        <v>31.15105628967285</v>
       </c>
       <c r="F61" t="n">
-        <v>0.967741935483871</v>
+        <v>0.9583333333333334</v>
       </c>
       <c r="G61" t="n">
         <v>1</v>
@@ -1789,16 +1789,16 @@
         <v>0.75</v>
       </c>
       <c r="C62" t="n">
-        <v>0.9885057471264368</v>
+        <v>0.9855072463768116</v>
       </c>
       <c r="D62" t="n">
         <v>0</v>
       </c>
       <c r="E62" t="n">
-        <v>30.10845184326172</v>
+        <v>36.00382804870605</v>
       </c>
       <c r="F62" t="n">
-        <v>0.9777777777777777</v>
+        <v>0.9722222222222222</v>
       </c>
       <c r="G62" t="n">
         <v>1</v>
@@ -1810,13 +1810,13 @@
         <v>0.95</v>
       </c>
       <c r="C63" t="n">
-        <v>1</v>
+        <v>0.9882352941176471</v>
       </c>
       <c r="D63" t="n">
         <v>0</v>
       </c>
       <c r="E63" t="n">
-        <v>37.12344169616699</v>
+        <v>50.72002410888671</v>
       </c>
       <c r="F63" t="n">
         <v>1</v>
@@ -1837,7 +1837,7 @@
         <v>0</v>
       </c>
       <c r="E64" t="n">
-        <v>170.8016395568848</v>
+        <v>128.5982131958008</v>
       </c>
       <c r="F64" t="n">
         <v>1</v>
@@ -1877,19 +1877,19 @@
         <v>0.05</v>
       </c>
       <c r="C66" t="n">
-        <v>0.8047378749649565</v>
+        <v>0.4232854864433812</v>
       </c>
       <c r="D66" t="n">
         <v>0</v>
       </c>
       <c r="E66" t="n">
-        <v>0</v>
+        <v>1.560807228088379</v>
       </c>
       <c r="F66" t="n">
-        <v>0.75</v>
+        <v>0.6848214285714286</v>
       </c>
       <c r="G66" t="n">
-        <v>0.96875</v>
+        <v>0.2846153846153846</v>
       </c>
     </row>
     <row r="67">
@@ -1898,19 +1898,19 @@
         <v>0.25</v>
       </c>
       <c r="C67" t="n">
-        <v>0.9811320754716981</v>
+        <v>0.8300000000000001</v>
       </c>
       <c r="D67" t="n">
         <v>0</v>
       </c>
       <c r="E67" t="n">
-        <v>3.173708915710449</v>
+        <v>2.992987632751465</v>
       </c>
       <c r="F67" t="n">
-        <v>0.967741935483871</v>
+        <v>0.9672043010752689</v>
       </c>
       <c r="G67" t="n">
-        <v>1</v>
+        <v>0.7936105476673427</v>
       </c>
     </row>
     <row r="68">
@@ -1919,16 +1919,16 @@
         <v>0.5</v>
       </c>
       <c r="C68" t="n">
-        <v>0.9887640449438202</v>
+        <v>0.9811320754716981</v>
       </c>
       <c r="D68" t="n">
         <v>0</v>
       </c>
       <c r="E68" t="n">
-        <v>3.991127014160156</v>
+        <v>3.988981246948242</v>
       </c>
       <c r="F68" t="n">
-        <v>0.9791666666666666</v>
+        <v>1</v>
       </c>
       <c r="G68" t="n">
         <v>1</v>
@@ -1946,7 +1946,7 @@
         <v>0</v>
       </c>
       <c r="E69" t="n">
-        <v>4.988908767700195</v>
+        <v>4.962682723999023</v>
       </c>
       <c r="F69" t="n">
         <v>1</v>
@@ -1967,7 +1967,7 @@
         <v>0</v>
       </c>
       <c r="E70" t="n">
-        <v>10.14125347137451</v>
+        <v>6.14309310913085</v>
       </c>
       <c r="F70" t="n">
         <v>1</v>
@@ -1988,7 +1988,7 @@
         <v>0</v>
       </c>
       <c r="E71" t="n">
-        <v>98.03247451782227</v>
+        <v>25.92921257019043</v>
       </c>
       <c r="F71" t="n">
         <v>1</v>
@@ -2028,19 +2028,19 @@
         <v>0.05</v>
       </c>
       <c r="C73" t="n">
-        <v>0.8145502645502645</v>
+        <v>0</v>
       </c>
       <c r="D73" t="n">
         <v>0</v>
       </c>
       <c r="E73" t="n">
-        <v>0</v>
+        <v>1.089262962341309</v>
       </c>
       <c r="F73" t="n">
-        <v>0.8333333333333334</v>
+        <v>0</v>
       </c>
       <c r="G73" t="n">
-        <v>0.9</v>
+        <v>0</v>
       </c>
     </row>
     <row r="74">
@@ -2049,19 +2049,19 @@
         <v>0.25</v>
       </c>
       <c r="C74" t="n">
-        <v>0.9795918367346939</v>
+        <v>0.2910628019323672</v>
       </c>
       <c r="D74" t="n">
         <v>0</v>
       </c>
       <c r="E74" t="n">
-        <v>1.994848251342773</v>
+        <v>1.99580192565918</v>
       </c>
       <c r="F74" t="n">
-        <v>0.972972972972973</v>
+        <v>0.3660714285714286</v>
       </c>
       <c r="G74" t="n">
-        <v>0.9767441860465116</v>
+        <v>0.205010775862069</v>
       </c>
     </row>
     <row r="75">
@@ -2070,19 +2070,19 @@
         <v>0.5</v>
       </c>
       <c r="C75" t="n">
-        <v>0.9879518072289156</v>
+        <v>0.9583333333333334</v>
       </c>
       <c r="D75" t="n">
         <v>0</v>
       </c>
       <c r="E75" t="n">
-        <v>2.991199493408203</v>
+        <v>2.991676330566406</v>
       </c>
       <c r="F75" t="n">
         <v>1</v>
       </c>
       <c r="G75" t="n">
-        <v>1</v>
+        <v>0.9399999999999999</v>
       </c>
     </row>
     <row r="76">
@@ -2091,13 +2091,13 @@
         <v>0.75</v>
       </c>
       <c r="C76" t="n">
-        <v>1</v>
+        <v>0.987878342638848</v>
       </c>
       <c r="D76" t="n">
         <v>0</v>
       </c>
       <c r="E76" t="n">
-        <v>3.020524978637695</v>
+        <v>3.46672534942627</v>
       </c>
       <c r="F76" t="n">
         <v>1</v>
@@ -2118,7 +2118,7 @@
         <v>0</v>
       </c>
       <c r="E77" t="n">
-        <v>5.353331565856934</v>
+        <v>4.960036277770994</v>
       </c>
       <c r="F77" t="n">
         <v>1</v>
@@ -2139,7 +2139,7 @@
         <v>0</v>
       </c>
       <c r="E78" t="n">
-        <v>133.7661743164062</v>
+        <v>7.542610168457031</v>
       </c>
       <c r="F78" t="n">
         <v>1</v>
@@ -2179,19 +2179,19 @@
         <v>0.05</v>
       </c>
       <c r="C80" t="n">
-        <v>0.8686868686868687</v>
+        <v>0</v>
       </c>
       <c r="D80" t="n">
         <v>0</v>
       </c>
       <c r="E80" t="n">
-        <v>3.24404239654541</v>
+        <v>8.764576911926273</v>
       </c>
       <c r="F80" t="n">
-        <v>0.8143841515934539</v>
+        <v>0</v>
       </c>
       <c r="G80" t="n">
-        <v>0.9714285714285714</v>
+        <v>0</v>
       </c>
     </row>
     <row r="81">
@@ -2200,19 +2200,19 @@
         <v>0.25</v>
       </c>
       <c r="C81" t="n">
-        <v>0.9850746268656716</v>
+        <v>0.8333333333333334</v>
       </c>
       <c r="D81" t="n">
         <v>0</v>
       </c>
       <c r="E81" t="n">
-        <v>10.96987724304199</v>
+        <v>13.40866088867188</v>
       </c>
       <c r="F81" t="n">
-        <v>0.972972972972973</v>
+        <v>0.9642857142857143</v>
       </c>
       <c r="G81" t="n">
-        <v>1</v>
+        <v>0.7575757575757576</v>
       </c>
     </row>
     <row r="82">
@@ -2221,13 +2221,13 @@
         <v>0.5</v>
       </c>
       <c r="C82" t="n">
-        <v>1</v>
+        <v>0.9824561403508771</v>
       </c>
       <c r="D82" t="n">
         <v>0</v>
       </c>
       <c r="E82" t="n">
-        <v>13.9315128326416</v>
+        <v>16.92461967468262</v>
       </c>
       <c r="F82" t="n">
         <v>1</v>
@@ -2248,7 +2248,7 @@
         <v>0</v>
       </c>
       <c r="E83" t="n">
-        <v>17.95220375061035</v>
+        <v>19.94979381561279</v>
       </c>
       <c r="F83" t="n">
         <v>1</v>
@@ -2269,7 +2269,7 @@
         <v>0</v>
       </c>
       <c r="E84" t="n">
-        <v>26.95858478546143</v>
+        <v>28.31723690032959</v>
       </c>
       <c r="F84" t="n">
         <v>1</v>
@@ -2290,7 +2290,7 @@
         <v>1</v>
       </c>
       <c r="E85" t="n">
-        <v>78639.72449302673</v>
+        <v>662.0008945465088</v>
       </c>
       <c r="F85" t="n">
         <v>1</v>
@@ -2330,19 +2330,19 @@
         <v>0.05</v>
       </c>
       <c r="C87" t="n">
-        <v>0.6605504587155964</v>
+        <v>0</v>
       </c>
       <c r="D87" t="n">
         <v>0</v>
       </c>
       <c r="E87" t="n">
-        <v>6.984710693359375</v>
+        <v>15.50219058990479</v>
       </c>
       <c r="F87" t="n">
-        <v>0.6141604010025064</v>
+        <v>0</v>
       </c>
       <c r="G87" t="n">
-        <v>0.6170212765957447</v>
+        <v>0</v>
       </c>
     </row>
     <row r="88">
@@ -2351,19 +2351,19 @@
         <v>0.25</v>
       </c>
       <c r="C88" t="n">
-        <v>0.9770992366412213</v>
+        <v>0.3601962741184298</v>
       </c>
       <c r="D88" t="n">
         <v>0</v>
       </c>
       <c r="E88" t="n">
-        <v>16.20876789093018</v>
+        <v>18.66769790649414</v>
       </c>
       <c r="F88" t="n">
-        <v>0.9837387625594923</v>
+        <v>0.90935192780968</v>
       </c>
       <c r="G88" t="n">
-        <v>1</v>
+        <v>0.2734572837531654</v>
       </c>
     </row>
     <row r="89">
@@ -2372,19 +2372,19 @@
         <v>0.5</v>
       </c>
       <c r="C89" t="n">
-        <v>1</v>
+        <v>0.8787878787878788</v>
       </c>
       <c r="D89" t="n">
         <v>0</v>
       </c>
       <c r="E89" t="n">
-        <v>18.92781257629395</v>
+        <v>21.09289169311523</v>
       </c>
       <c r="F89" t="n">
         <v>1</v>
       </c>
       <c r="G89" t="n">
-        <v>1</v>
+        <v>0.8333333333333334</v>
       </c>
     </row>
     <row r="90">
@@ -2399,7 +2399,7 @@
         <v>0</v>
       </c>
       <c r="E90" t="n">
-        <v>21.9426155090332</v>
+        <v>23.22590351104736</v>
       </c>
       <c r="F90" t="n">
         <v>1</v>
@@ -2420,7 +2420,7 @@
         <v>0</v>
       </c>
       <c r="E91" t="n">
-        <v>30.69961071014404</v>
+        <v>27.9299259185791</v>
       </c>
       <c r="F91" t="n">
         <v>1</v>
@@ -2441,7 +2441,7 @@
         <v>1</v>
       </c>
       <c r="E92" t="n">
-        <v>357117.9120540619</v>
+        <v>172.8610992431641</v>
       </c>
       <c r="F92" t="n">
         <v>1</v>
@@ -2481,19 +2481,19 @@
         <v>0.05</v>
       </c>
       <c r="C94" t="n">
-        <v>0.875</v>
+        <v>0.3621428571428572</v>
       </c>
       <c r="D94" t="n">
         <v>0</v>
       </c>
       <c r="E94" t="n">
-        <v>0</v>
+        <v>3.989696502685547</v>
       </c>
       <c r="F94" t="n">
-        <v>0.8846153846153846</v>
+        <v>0.9135416666666667</v>
       </c>
       <c r="G94" t="n">
-        <v>0.9444444444444444</v>
+        <v>0.2264033264033264</v>
       </c>
     </row>
     <row r="95">
@@ -2502,19 +2502,19 @@
         <v>0.25</v>
       </c>
       <c r="C95" t="n">
-        <v>0.9830508474576272</v>
+        <v>0.8207949696833595</v>
       </c>
       <c r="D95" t="n">
         <v>0</v>
       </c>
       <c r="E95" t="n">
-        <v>3.97956371307373</v>
+        <v>6.02412223815918</v>
       </c>
       <c r="F95" t="n">
-        <v>0.9722222222222222</v>
+        <v>0.9789450354609929</v>
       </c>
       <c r="G95" t="n">
-        <v>1</v>
+        <v>0.717670011148272</v>
       </c>
     </row>
     <row r="96">
@@ -2523,13 +2523,13 @@
         <v>0.5</v>
       </c>
       <c r="C96" t="n">
-        <v>0.9898989898989899</v>
+        <v>0.9818181818181818</v>
       </c>
       <c r="D96" t="n">
         <v>0</v>
       </c>
       <c r="E96" t="n">
-        <v>5.980968475341797</v>
+        <v>8.018255233764648</v>
       </c>
       <c r="F96" t="n">
         <v>1</v>
@@ -2550,7 +2550,7 @@
         <v>0</v>
       </c>
       <c r="E97" t="n">
-        <v>8.97669792175293</v>
+        <v>10.10191440582275</v>
       </c>
       <c r="F97" t="n">
         <v>1</v>
@@ -2571,7 +2571,7 @@
         <v>0</v>
       </c>
       <c r="E98" t="n">
-        <v>18.90277862548828</v>
+        <v>13.97163867950439</v>
       </c>
       <c r="F98" t="n">
         <v>1</v>
@@ -2592,7 +2592,7 @@
         <v>0</v>
       </c>
       <c r="E99" t="n">
-        <v>54.84485626220703</v>
+        <v>40.64726829528809</v>
       </c>
       <c r="F99" t="n">
         <v>1</v>
@@ -2617,7 +2617,7 @@
         <v>0</v>
       </c>
       <c r="E100" t="n">
-        <v>10.0395679473877</v>
+        <v>23.79775047302246</v>
       </c>
       <c r="F100" t="n">
         <v>0</v>
@@ -2632,19 +2632,19 @@
         <v>0.05</v>
       </c>
       <c r="C101" t="n">
-        <v>0.7965351732413379</v>
+        <v>0.4130150173276858</v>
       </c>
       <c r="D101" t="n">
         <v>0</v>
       </c>
       <c r="E101" t="n">
-        <v>22.93968200683594</v>
+        <v>29.59902286529541</v>
       </c>
       <c r="F101" t="n">
-        <v>0.875</v>
+        <v>0.9143939393939394</v>
       </c>
       <c r="G101" t="n">
-        <v>0.8934873949579832</v>
+        <v>0.2647279549718575</v>
       </c>
     </row>
     <row r="102">
@@ -2653,19 +2653,19 @@
         <v>0.25</v>
       </c>
       <c r="C102" t="n">
-        <v>0.9859154929577465</v>
+        <v>0.8452991452991453</v>
       </c>
       <c r="D102" t="n">
         <v>0</v>
       </c>
       <c r="E102" t="n">
-        <v>27.5886058807373</v>
+        <v>32.86218643188477</v>
       </c>
       <c r="F102" t="n">
-        <v>0.98</v>
+        <v>1</v>
       </c>
       <c r="G102" t="n">
-        <v>1</v>
+        <v>0.7464285714285714</v>
       </c>
     </row>
     <row r="103">
@@ -2674,13 +2674,13 @@
         <v>0.5</v>
       </c>
       <c r="C103" t="n">
-        <v>1</v>
+        <v>0.9859154929577465</v>
       </c>
       <c r="D103" t="n">
         <v>0</v>
       </c>
       <c r="E103" t="n">
-        <v>32.37700462341309</v>
+        <v>40.01116752624512</v>
       </c>
       <c r="F103" t="n">
         <v>1</v>
@@ -2701,7 +2701,7 @@
         <v>0</v>
       </c>
       <c r="E104" t="n">
-        <v>37.33062744140625</v>
+        <v>53.99167537689209</v>
       </c>
       <c r="F104" t="n">
         <v>1</v>
@@ -2722,7 +2722,7 @@
         <v>0</v>
       </c>
       <c r="E105" t="n">
-        <v>49.78299140930176</v>
+        <v>80.77621459960935</v>
       </c>
       <c r="F105" t="n">
         <v>1</v>
@@ -2743,7 +2743,7 @@
         <v>0</v>
       </c>
       <c r="E106" t="n">
-        <v>20262.54224777222</v>
+        <v>393.5410976409912</v>
       </c>
       <c r="F106" t="n">
         <v>1</v>
@@ -2768,7 +2768,7 @@
         <v>0</v>
       </c>
       <c r="E107" t="n">
-        <v>75.12402534484863</v>
+        <v>88.8063907623291</v>
       </c>
       <c r="F107" t="n">
         <v>0</v>
@@ -2783,19 +2783,19 @@
         <v>0.05</v>
       </c>
       <c r="C108" t="n">
-        <v>0.6736842105263158</v>
+        <v>0.2823529411764706</v>
       </c>
       <c r="D108" t="n">
         <v>0</v>
       </c>
       <c r="E108" t="n">
-        <v>90.76309204101562</v>
+        <v>169.935941696167</v>
       </c>
       <c r="F108" t="n">
-        <v>0.8802985074626866</v>
+        <v>0.6207407407407408</v>
       </c>
       <c r="G108" t="n">
-        <v>0.509090909090909</v>
+        <v>0.1953194180898166</v>
       </c>
     </row>
     <row r="109">
@@ -2804,19 +2804,19 @@
         <v>0.25</v>
       </c>
       <c r="C109" t="n">
-        <v>0.9122807017543859</v>
+        <v>0.7097222222222223</v>
       </c>
       <c r="D109" t="n">
         <v>0</v>
       </c>
       <c r="E109" t="n">
-        <v>110.7029914855957</v>
+        <v>243.1625127792358</v>
       </c>
       <c r="F109" t="n">
-        <v>1</v>
+        <v>0.9652147610405324</v>
       </c>
       <c r="G109" t="n">
-        <v>0.8958333333333334</v>
+        <v>0.5816666666666667</v>
       </c>
     </row>
     <row r="110">
@@ -2825,19 +2825,19 @@
         <v>0.5</v>
       </c>
       <c r="C110" t="n">
-        <v>0.9855072463768116</v>
+        <v>0.8732394366197183</v>
       </c>
       <c r="D110" t="n">
         <v>0</v>
       </c>
       <c r="E110" t="n">
-        <v>189.1820430755615</v>
+        <v>280.7493209838867</v>
       </c>
       <c r="F110" t="n">
         <v>1</v>
       </c>
       <c r="G110" t="n">
-        <v>0.975</v>
+        <v>0.8108108108108109</v>
       </c>
     </row>
     <row r="111">
@@ -2846,19 +2846,19 @@
         <v>0.75</v>
       </c>
       <c r="C111" t="n">
-        <v>0.9908256880733946</v>
+        <v>0.9855072463768116</v>
       </c>
       <c r="D111" t="n">
         <v>0</v>
       </c>
       <c r="E111" t="n">
-        <v>274.3216753005981</v>
+        <v>357.7612638473511</v>
       </c>
       <c r="F111" t="n">
         <v>1</v>
       </c>
       <c r="G111" t="n">
-        <v>1</v>
+        <v>0.9722222222222222</v>
       </c>
     </row>
     <row r="112">
@@ -2867,13 +2867,13 @@
         <v>0.95</v>
       </c>
       <c r="C112" t="n">
-        <v>1</v>
+        <v>0.9911504424778761</v>
       </c>
       <c r="D112" t="n">
         <v>0</v>
       </c>
       <c r="E112" t="n">
-        <v>344.5345163345337</v>
+        <v>451.9218683242794</v>
       </c>
       <c r="F112" t="n">
         <v>1</v>
@@ -2894,7 +2894,7 @@
         <v>0</v>
       </c>
       <c r="E113" t="n">
-        <v>1114.78853225708</v>
+        <v>620.9404468536377</v>
       </c>
       <c r="F113" t="n">
         <v>1</v>

</xml_diff>

<commit_message>
adjusted main_pc to re-run analysis of ARR and SIN databases
Previously recordings in these databases were skipped if they had been run before.
</commit_message>
<xml_diff>
--- a/Algorithm_tester/data_autosave/real_overall.xlsx
+++ b/Algorithm_tester/data_autosave/real_overall.xlsx
@@ -446,7 +446,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G113"/>
+  <dimension ref="A1:H113"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -486,6 +486,11 @@
           <t>positive_predictivity</t>
         </is>
       </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>heart_rate</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
@@ -503,12 +508,15 @@
         <v>0</v>
       </c>
       <c r="E2" t="n">
-        <v>92.09895133972168</v>
+        <v>60.35780906677246</v>
       </c>
       <c r="F2" t="n">
         <v>0</v>
       </c>
       <c r="G2" t="n">
+        <v>0</v>
+      </c>
+      <c r="H2" t="n">
         <v>0</v>
       </c>
     </row>
@@ -518,19 +526,22 @@
         <v>0.05</v>
       </c>
       <c r="C3" t="n">
-        <v>0</v>
+        <v>0.05171052631578948</v>
       </c>
       <c r="D3" t="n">
         <v>0</v>
       </c>
       <c r="E3" t="n">
-        <v>166.1584377288818</v>
+        <v>111.6964221000671</v>
       </c>
       <c r="F3" t="n">
-        <v>0</v>
+        <v>0.04516885553470926</v>
       </c>
       <c r="G3" t="n">
-        <v>0</v>
+        <v>0.1156828020464384</v>
+      </c>
+      <c r="H3" t="n">
+        <v>29.99700029997</v>
       </c>
     </row>
     <row r="4">
@@ -539,19 +550,22 @@
         <v>0.25</v>
       </c>
       <c r="C4" t="n">
-        <v>0.4267857142857143</v>
+        <v>0.4546815459989113</v>
       </c>
       <c r="D4" t="n">
         <v>0</v>
       </c>
       <c r="E4" t="n">
-        <v>188.88258934021</v>
+        <v>156.716525554657</v>
       </c>
       <c r="F4" t="n">
-        <v>0.9714285714285714</v>
+        <v>0.9736842105263158</v>
       </c>
       <c r="G4" t="n">
-        <v>0.2862997658079625</v>
+        <v>0.3044327445652174</v>
+      </c>
+      <c r="H4" t="n">
+        <v>60</v>
       </c>
     </row>
     <row r="5">
@@ -560,19 +574,22 @@
         <v>0.5</v>
       </c>
       <c r="C5" t="n">
-        <v>0.9411764705882353</v>
+        <v>0.7703296703296704</v>
       </c>
       <c r="D5" t="n">
         <v>0</v>
       </c>
       <c r="E5" t="n">
-        <v>249.0637302398682</v>
+        <v>197.9329586029053</v>
       </c>
       <c r="F5" t="n">
         <v>1</v>
       </c>
       <c r="G5" t="n">
-        <v>0.9375</v>
+        <v>0.6812893081761007</v>
+      </c>
+      <c r="H5" t="n">
+        <v>72.0096012801707</v>
       </c>
     </row>
     <row r="6">
@@ -581,19 +598,22 @@
         <v>0.75</v>
       </c>
       <c r="C6" t="n">
-        <v>0.9866666666666667</v>
+        <v>0.9850746268656716</v>
       </c>
       <c r="D6" t="n">
         <v>0</v>
       </c>
       <c r="E6" t="n">
-        <v>295.1279878616333</v>
+        <v>211.6356492042542</v>
       </c>
       <c r="F6" t="n">
         <v>1</v>
       </c>
       <c r="G6" t="n">
-        <v>1</v>
+        <v>0.9767441860465116</v>
+      </c>
+      <c r="H6" t="n">
+        <v>85.88309518125703</v>
       </c>
     </row>
     <row r="7">
@@ -608,13 +628,16 @@
         <v>0</v>
       </c>
       <c r="E7" t="n">
-        <v>401.4069318771362</v>
+        <v>230.163586139679</v>
       </c>
       <c r="F7" t="n">
         <v>1</v>
       </c>
       <c r="G7" t="n">
         <v>1</v>
+      </c>
+      <c r="H7" t="n">
+        <v>114</v>
       </c>
     </row>
     <row r="8">
@@ -629,13 +652,16 @@
         <v>0</v>
       </c>
       <c r="E8" t="n">
-        <v>625.4055500030518</v>
+        <v>252.3441314697266</v>
       </c>
       <c r="F8" t="n">
         <v>1</v>
       </c>
       <c r="G8" t="n">
         <v>1</v>
+      </c>
+      <c r="H8" t="n">
+        <v>168</v>
       </c>
     </row>
     <row r="9">
@@ -662,6 +688,9 @@
       <c r="G9" t="n">
         <v>0</v>
       </c>
+      <c r="H9" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="10">
       <c r="A10" s="1" t="n"/>
@@ -683,6 +712,9 @@
       <c r="G10" t="n">
         <v>0</v>
       </c>
+      <c r="H10" t="n">
+        <v>29.99700029997</v>
+      </c>
     </row>
     <row r="11">
       <c r="A11" s="1" t="n"/>
@@ -690,19 +722,22 @@
         <v>0.25</v>
       </c>
       <c r="C11" t="n">
-        <v>0</v>
+        <v>0.1482176360225141</v>
       </c>
       <c r="D11" t="n">
         <v>0</v>
       </c>
       <c r="E11" t="n">
-        <v>64.78762626647949</v>
+        <v>47.7641224861145</v>
       </c>
       <c r="F11" t="n">
-        <v>0</v>
+        <v>0.08522727272727272</v>
       </c>
       <c r="G11" t="n">
-        <v>0</v>
+        <v>0.5244360902255639</v>
+      </c>
+      <c r="H11" t="n">
+        <v>60</v>
       </c>
     </row>
     <row r="12">
@@ -711,19 +746,22 @@
         <v>0.5</v>
       </c>
       <c r="C12" t="n">
-        <v>0.7951807228915663</v>
+        <v>0.6666666666666666</v>
       </c>
       <c r="D12" t="n">
         <v>0</v>
       </c>
       <c r="E12" t="n">
-        <v>86.65943145751953</v>
+        <v>67.58248805999756</v>
       </c>
       <c r="F12" t="n">
-        <v>0.7586206896551724</v>
+        <v>0.5384615384615384</v>
       </c>
       <c r="G12" t="n">
         <v>1</v>
+      </c>
+      <c r="H12" t="n">
+        <v>72.0096012801707</v>
       </c>
     </row>
     <row r="13">
@@ -732,19 +770,22 @@
         <v>0.75</v>
       </c>
       <c r="C13" t="n">
-        <v>0.9830508474576272</v>
+        <v>0.952921157118548</v>
       </c>
       <c r="D13" t="n">
         <v>0</v>
       </c>
       <c r="E13" t="n">
-        <v>101.6875505447388</v>
+        <v>84.20681953430176</v>
       </c>
       <c r="F13" t="n">
-        <v>0.9701426024955437</v>
+        <v>0.9266034327009938</v>
       </c>
       <c r="G13" t="n">
         <v>1</v>
+      </c>
+      <c r="H13" t="n">
+        <v>85.88309518125703</v>
       </c>
     </row>
     <row r="14">
@@ -759,13 +800,16 @@
         <v>1</v>
       </c>
       <c r="E14" t="n">
-        <v>138.3724927902221</v>
+        <v>93.55617761611938</v>
       </c>
       <c r="F14" t="n">
-        <v>0.9782608695652174</v>
+        <v>0.9772727272727273</v>
       </c>
       <c r="G14" t="n">
         <v>1</v>
+      </c>
+      <c r="H14" t="n">
+        <v>114</v>
       </c>
     </row>
     <row r="15">
@@ -780,13 +824,16 @@
         <v>1</v>
       </c>
       <c r="E15" t="n">
-        <v>215.8746719360352</v>
+        <v>156.6369533538818</v>
       </c>
       <c r="F15" t="n">
         <v>1</v>
       </c>
       <c r="G15" t="n">
         <v>1</v>
+      </c>
+      <c r="H15" t="n">
+        <v>168</v>
       </c>
     </row>
     <row r="16">
@@ -813,6 +860,9 @@
       <c r="G16" t="n">
         <v>0</v>
       </c>
+      <c r="H16" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="17">
       <c r="A17" s="1" t="n"/>
@@ -820,19 +870,22 @@
         <v>0.05</v>
       </c>
       <c r="C17" t="n">
-        <v>0.2888888888888889</v>
+        <v>0</v>
       </c>
       <c r="D17" t="n">
         <v>0</v>
       </c>
       <c r="E17" t="n">
-        <v>4.849863052368164</v>
+        <v>0</v>
       </c>
       <c r="F17" t="n">
-        <v>0.9597551020408163</v>
+        <v>0</v>
       </c>
       <c r="G17" t="n">
-        <v>0.1688311688311688</v>
+        <v>0</v>
+      </c>
+      <c r="H17" t="n">
+        <v>29.99700029997</v>
       </c>
     </row>
     <row r="18">
@@ -841,19 +894,22 @@
         <v>0.25</v>
       </c>
       <c r="C18" t="n">
-        <v>0.5102040816326531</v>
+        <v>0</v>
       </c>
       <c r="D18" t="n">
         <v>0</v>
       </c>
       <c r="E18" t="n">
-        <v>6.972312927246094</v>
+        <v>0</v>
       </c>
       <c r="F18" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G18" t="n">
-        <v>0.3443533697632059</v>
+        <v>0</v>
+      </c>
+      <c r="H18" t="n">
+        <v>60</v>
       </c>
     </row>
     <row r="19">
@@ -862,19 +918,22 @@
         <v>0.5</v>
       </c>
       <c r="C19" t="n">
-        <v>0.5909090909090909</v>
+        <v>0.4196009389671361</v>
       </c>
       <c r="D19" t="n">
         <v>0</v>
       </c>
       <c r="E19" t="n">
-        <v>10.42509078979492</v>
+        <v>1.990437507629395</v>
       </c>
       <c r="F19" t="n">
-        <v>1</v>
+        <v>0.9074074074074074</v>
       </c>
       <c r="G19" t="n">
-        <v>0.4197530864197531</v>
+        <v>0.2655075187969925</v>
+      </c>
+      <c r="H19" t="n">
+        <v>72.0096012801707</v>
       </c>
     </row>
     <row r="20">
@@ -883,19 +942,22 @@
         <v>0.75</v>
       </c>
       <c r="C20" t="n">
-        <v>0.6610869869729654</v>
+        <v>0.6322537112010795</v>
       </c>
       <c r="D20" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E20" t="n">
-        <v>18.05734634399414</v>
+        <v>2.715766429901123</v>
       </c>
       <c r="F20" t="n">
         <v>1</v>
       </c>
       <c r="G20" t="n">
-        <v>0.4941045914828686</v>
+        <v>0.4625</v>
+      </c>
+      <c r="H20" t="n">
+        <v>85.88309518125703</v>
       </c>
     </row>
     <row r="21">
@@ -904,19 +966,22 @@
         <v>0.95</v>
       </c>
       <c r="C21" t="n">
-        <v>0.8</v>
+        <v>0.8343939393939391</v>
       </c>
       <c r="D21" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E21" t="n">
-        <v>89.62256908416747</v>
+        <v>5.116319656372069</v>
       </c>
       <c r="F21" t="n">
         <v>1</v>
       </c>
       <c r="G21" t="n">
-        <v>0.6678861788617885</v>
+        <v>0.7231944444444441</v>
+      </c>
+      <c r="H21" t="n">
+        <v>114</v>
       </c>
     </row>
     <row r="22">
@@ -925,19 +990,22 @@
         <v>1</v>
       </c>
       <c r="C22" t="n">
-        <v>0.9642857142857143</v>
+        <v>1</v>
       </c>
       <c r="D22" t="n">
         <v>1</v>
       </c>
       <c r="E22" t="n">
-        <v>280.9844017028809</v>
+        <v>78.72581481933594</v>
       </c>
       <c r="F22" t="n">
         <v>1</v>
       </c>
       <c r="G22" t="n">
-        <v>0.9310344827586207</v>
+        <v>1</v>
+      </c>
+      <c r="H22" t="n">
+        <v>168</v>
       </c>
     </row>
     <row r="23">
@@ -956,12 +1024,15 @@
         <v>0</v>
       </c>
       <c r="E23" t="n">
-        <v>51.86057090759277</v>
+        <v>0</v>
       </c>
       <c r="F23" t="n">
         <v>0</v>
       </c>
       <c r="G23" t="n">
+        <v>0</v>
+      </c>
+      <c r="H23" t="n">
         <v>0</v>
       </c>
     </row>
@@ -971,19 +1042,22 @@
         <v>0.05</v>
       </c>
       <c r="C24" t="n">
-        <v>0.3709914320685435</v>
+        <v>0.4722442244224423</v>
       </c>
       <c r="D24" t="n">
         <v>0</v>
       </c>
       <c r="E24" t="n">
-        <v>91.00511074066162</v>
+        <v>62.21141815185547</v>
       </c>
       <c r="F24" t="n">
-        <v>0.6506393861892583</v>
+        <v>0.7145909090909092</v>
       </c>
       <c r="G24" t="n">
-        <v>0.2484693877551021</v>
+        <v>0.3182739726027398</v>
+      </c>
+      <c r="H24" t="n">
+        <v>29.99700029997</v>
       </c>
     </row>
     <row r="25">
@@ -992,19 +1066,22 @@
         <v>0.25</v>
       </c>
       <c r="C25" t="n">
-        <v>0.8155706727135299</v>
+        <v>0.6666666666666666</v>
       </c>
       <c r="D25" t="n">
         <v>0</v>
       </c>
       <c r="E25" t="n">
-        <v>118.0760860443115</v>
+        <v>88.17487955093384</v>
       </c>
       <c r="F25" t="n">
-        <v>0.9603921568627451</v>
+        <v>0.972972972972973</v>
       </c>
       <c r="G25" t="n">
-        <v>0.7565656565656566</v>
+        <v>0.5068493150684932</v>
+      </c>
+      <c r="H25" t="n">
+        <v>60</v>
       </c>
     </row>
     <row r="26">
@@ -1013,19 +1090,22 @@
         <v>0.5</v>
       </c>
       <c r="C26" t="n">
-        <v>0.9662921348314607</v>
+        <v>0.8489256639530228</v>
       </c>
       <c r="D26" t="n">
         <v>0</v>
       </c>
       <c r="E26" t="n">
-        <v>141.803503036499</v>
+        <v>121.5285062789917</v>
       </c>
       <c r="F26" t="n">
         <v>1</v>
       </c>
       <c r="G26" t="n">
-        <v>1</v>
+        <v>0.8636363636363636</v>
+      </c>
+      <c r="H26" t="n">
+        <v>72.0096012801707</v>
       </c>
     </row>
     <row r="27">
@@ -1034,19 +1114,22 @@
         <v>0.75</v>
       </c>
       <c r="C27" t="n">
-        <v>1</v>
+        <v>0.9906542056074766</v>
       </c>
       <c r="D27" t="n">
         <v>0</v>
       </c>
       <c r="E27" t="n">
-        <v>172.5533008575439</v>
+        <v>133.4934234619141</v>
       </c>
       <c r="F27" t="n">
         <v>1</v>
       </c>
       <c r="G27" t="n">
         <v>1</v>
+      </c>
+      <c r="H27" t="n">
+        <v>85.88309518125703</v>
       </c>
     </row>
     <row r="28">
@@ -1061,13 +1144,16 @@
         <v>0</v>
       </c>
       <c r="E28" t="n">
-        <v>256.2325239181518</v>
+        <v>142.6933765411377</v>
       </c>
       <c r="F28" t="n">
         <v>1</v>
       </c>
       <c r="G28" t="n">
         <v>1</v>
+      </c>
+      <c r="H28" t="n">
+        <v>114</v>
       </c>
     </row>
     <row r="29">
@@ -1079,16 +1165,19 @@
         <v>1</v>
       </c>
       <c r="D29" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E29" t="n">
-        <v>434.6280097961426</v>
+        <v>156.9509506225586</v>
       </c>
       <c r="F29" t="n">
         <v>1</v>
       </c>
       <c r="G29" t="n">
         <v>1</v>
+      </c>
+      <c r="H29" t="n">
+        <v>168</v>
       </c>
     </row>
     <row r="30">
@@ -1107,12 +1196,15 @@
         <v>0</v>
       </c>
       <c r="E30" t="n">
-        <v>7.108211517333984</v>
+        <v>-36.56482696533203</v>
       </c>
       <c r="F30" t="n">
         <v>0</v>
       </c>
       <c r="G30" t="n">
+        <v>0</v>
+      </c>
+      <c r="H30" t="n">
         <v>0</v>
       </c>
     </row>
@@ -1128,13 +1220,16 @@
         <v>0</v>
       </c>
       <c r="E31" t="n">
-        <v>9.895062446594238</v>
+        <v>8.170735836029053</v>
       </c>
       <c r="F31" t="n">
         <v>0</v>
       </c>
       <c r="G31" t="n">
         <v>0</v>
+      </c>
+      <c r="H31" t="n">
+        <v>29.99700029997</v>
       </c>
     </row>
     <row r="32">
@@ -1143,19 +1238,22 @@
         <v>0.25</v>
       </c>
       <c r="C32" t="n">
-        <v>0.3385416666666666</v>
+        <v>0.7444140446876425</v>
       </c>
       <c r="D32" t="n">
         <v>0</v>
       </c>
       <c r="E32" t="n">
-        <v>12.96460628509521</v>
+        <v>11.03270053863525</v>
       </c>
       <c r="F32" t="n">
-        <v>0.7336719883889695</v>
+        <v>0.976328903654485</v>
       </c>
       <c r="G32" t="n">
-        <v>0.244047619047619</v>
+        <v>0.6205555555555555</v>
+      </c>
+      <c r="H32" t="n">
+        <v>60</v>
       </c>
     </row>
     <row r="33">
@@ -1164,19 +1262,22 @@
         <v>0.5</v>
       </c>
       <c r="C33" t="n">
-        <v>0.9473684210526315</v>
+        <v>0.9536672629695886</v>
       </c>
       <c r="D33" t="n">
         <v>0</v>
       </c>
       <c r="E33" t="n">
-        <v>18.0671215057373</v>
+        <v>16.98446273803711</v>
       </c>
       <c r="F33" t="n">
         <v>1</v>
       </c>
       <c r="G33" t="n">
-        <v>0.9090909090909091</v>
+        <v>0.9230769230769231</v>
+      </c>
+      <c r="H33" t="n">
+        <v>72.0096012801707</v>
       </c>
     </row>
     <row r="34">
@@ -1185,19 +1286,22 @@
         <v>0.75</v>
       </c>
       <c r="C34" t="n">
-        <v>0.9863013698630136</v>
+        <v>0.9855072463768116</v>
       </c>
       <c r="D34" t="n">
         <v>0</v>
       </c>
       <c r="E34" t="n">
-        <v>23.93579483032227</v>
+        <v>19.25581693649292</v>
       </c>
       <c r="F34" t="n">
         <v>1</v>
       </c>
       <c r="G34" t="n">
-        <v>0.9761904761904762</v>
+        <v>0.9741902834008097</v>
+      </c>
+      <c r="H34" t="n">
+        <v>85.88309518125703</v>
       </c>
     </row>
     <row r="35">
@@ -1212,13 +1316,16 @@
         <v>0</v>
       </c>
       <c r="E35" t="n">
-        <v>34.50999259948729</v>
+        <v>21.28853797912598</v>
       </c>
       <c r="F35" t="n">
         <v>1</v>
       </c>
       <c r="G35" t="n">
         <v>1</v>
+      </c>
+      <c r="H35" t="n">
+        <v>114</v>
       </c>
     </row>
     <row r="36">
@@ -1233,13 +1340,16 @@
         <v>0</v>
       </c>
       <c r="E36" t="n">
-        <v>83.41193199157715</v>
+        <v>33.75625610351562</v>
       </c>
       <c r="F36" t="n">
         <v>1</v>
       </c>
       <c r="G36" t="n">
         <v>1</v>
+      </c>
+      <c r="H36" t="n">
+        <v>168</v>
       </c>
     </row>
     <row r="37">
@@ -1266,6 +1376,9 @@
       <c r="G37" t="n">
         <v>0</v>
       </c>
+      <c r="H37" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="38">
       <c r="A38" s="1" t="n"/>
@@ -1273,19 +1386,22 @@
         <v>0.05</v>
       </c>
       <c r="C38" t="n">
-        <v>0</v>
+        <v>0.1765151515151516</v>
       </c>
       <c r="D38" t="n">
         <v>0</v>
       </c>
       <c r="E38" t="n">
-        <v>9.525275230407715</v>
+        <v>1.493000000470784</v>
       </c>
       <c r="F38" t="n">
-        <v>0</v>
+        <v>0.1</v>
       </c>
       <c r="G38" t="n">
-        <v>0</v>
+        <v>0.3280303030303031</v>
+      </c>
+      <c r="H38" t="n">
+        <v>29.99700029997</v>
       </c>
     </row>
     <row r="39">
@@ -1294,19 +1410,22 @@
         <v>0.25</v>
       </c>
       <c r="C39" t="n">
-        <v>0.6402157164869029</v>
+        <v>0.7399797057331303</v>
       </c>
       <c r="D39" t="n">
         <v>0</v>
       </c>
       <c r="E39" t="n">
-        <v>12.64822483062744</v>
+        <v>2.589000001549721</v>
       </c>
       <c r="F39" t="n">
-        <v>0.6561913696060038</v>
+        <v>0.647456279809221</v>
       </c>
       <c r="G39" t="n">
-        <v>0.7609523809523809</v>
+        <v>0.9565217391304348</v>
+      </c>
+      <c r="H39" t="n">
+        <v>60</v>
       </c>
     </row>
     <row r="40">
@@ -1315,19 +1434,22 @@
         <v>0.5</v>
       </c>
       <c r="C40" t="n">
-        <v>0.9152542372881356</v>
+        <v>0.9459459459459459</v>
       </c>
       <c r="D40" t="n">
         <v>0</v>
       </c>
       <c r="E40" t="n">
-        <v>15.9294605255127</v>
+        <v>3.050999999046326</v>
       </c>
       <c r="F40" t="n">
-        <v>0.9705882352941176</v>
+        <v>0.9375</v>
       </c>
       <c r="G40" t="n">
-        <v>1</v>
+        <v>0.9743589743589743</v>
+      </c>
+      <c r="H40" t="n">
+        <v>72.0096012801707</v>
       </c>
     </row>
     <row r="41">
@@ -1336,19 +1458,22 @@
         <v>0.75</v>
       </c>
       <c r="C41" t="n">
-        <v>1</v>
+        <v>0.9875761837787154</v>
       </c>
       <c r="D41" t="n">
         <v>0</v>
       </c>
       <c r="E41" t="n">
-        <v>18.31746101379395</v>
+        <v>3.282750001177192</v>
       </c>
       <c r="F41" t="n">
         <v>1</v>
       </c>
       <c r="G41" t="n">
         <v>1</v>
+      </c>
+      <c r="H41" t="n">
+        <v>85.88309518125703</v>
       </c>
     </row>
     <row r="42">
@@ -1363,13 +1488,16 @@
         <v>0</v>
       </c>
       <c r="E42" t="n">
-        <v>23.61953258514402</v>
+        <v>3.930449997819959</v>
       </c>
       <c r="F42" t="n">
         <v>1</v>
       </c>
       <c r="G42" t="n">
         <v>1</v>
+      </c>
+      <c r="H42" t="n">
+        <v>114</v>
       </c>
     </row>
     <row r="43">
@@ -1384,13 +1512,16 @@
         <v>1</v>
       </c>
       <c r="E43" t="n">
-        <v>744.5070743560791</v>
+        <v>48.47800000011921</v>
       </c>
       <c r="F43" t="n">
         <v>1</v>
       </c>
       <c r="G43" t="n">
         <v>1</v>
+      </c>
+      <c r="H43" t="n">
+        <v>168</v>
       </c>
     </row>
     <row r="44">
@@ -1409,12 +1540,15 @@
         <v>0</v>
       </c>
       <c r="E44" t="n">
-        <v>0</v>
+        <v>1.666069030761719</v>
       </c>
       <c r="F44" t="n">
         <v>0</v>
       </c>
       <c r="G44" t="n">
+        <v>0</v>
+      </c>
+      <c r="H44" t="n">
         <v>0</v>
       </c>
     </row>
@@ -1430,13 +1564,16 @@
         <v>0</v>
       </c>
       <c r="E45" t="n">
-        <v>0.7397174835205103</v>
+        <v>1.889228820800781</v>
       </c>
       <c r="F45" t="n">
         <v>0</v>
       </c>
       <c r="G45" t="n">
         <v>0</v>
+      </c>
+      <c r="H45" t="n">
+        <v>29.99700029997</v>
       </c>
     </row>
     <row r="46">
@@ -1445,19 +1582,22 @@
         <v>0.25</v>
       </c>
       <c r="C46" t="n">
-        <v>0.2253968253968254</v>
+        <v>0.6666666666666666</v>
       </c>
       <c r="D46" t="n">
         <v>0</v>
       </c>
       <c r="E46" t="n">
-        <v>1.999139785766602</v>
+        <v>2.079963684082031</v>
       </c>
       <c r="F46" t="n">
-        <v>0.3452380952380952</v>
+        <v>0.8636363636363636</v>
       </c>
       <c r="G46" t="n">
-        <v>0.1726708074534161</v>
+        <v>0.5471698113207547</v>
+      </c>
+      <c r="H46" t="n">
+        <v>60</v>
       </c>
     </row>
     <row r="47">
@@ -1466,19 +1606,22 @@
         <v>0.5</v>
       </c>
       <c r="C47" t="n">
-        <v>0.9538461538461539</v>
+        <v>0.8888888888888888</v>
       </c>
       <c r="D47" t="n">
         <v>0</v>
       </c>
       <c r="E47" t="n">
-        <v>2.991437911987305</v>
+        <v>2.283573150634766</v>
       </c>
       <c r="F47" t="n">
-        <v>0.9795918367346939</v>
+        <v>0.9767441860465116</v>
       </c>
       <c r="G47" t="n">
-        <v>0.9444444444444444</v>
+        <v>0.8333333333333334</v>
+      </c>
+      <c r="H47" t="n">
+        <v>72.0096012801707</v>
       </c>
     </row>
     <row r="48">
@@ -1487,19 +1630,22 @@
         <v>0.75</v>
       </c>
       <c r="C48" t="n">
-        <v>0.9890109890109891</v>
+        <v>0.9859154929577465</v>
       </c>
       <c r="D48" t="n">
         <v>0</v>
       </c>
       <c r="E48" t="n">
-        <v>2.994894981384277</v>
+        <v>2.429723739624023</v>
       </c>
       <c r="F48" t="n">
         <v>1</v>
       </c>
       <c r="G48" t="n">
         <v>1</v>
+      </c>
+      <c r="H48" t="n">
+        <v>85.88309518125703</v>
       </c>
     </row>
     <row r="49">
@@ -1514,13 +1660,16 @@
         <v>0</v>
       </c>
       <c r="E49" t="n">
-        <v>4.003477096557615</v>
+        <v>4.243230819702148</v>
       </c>
       <c r="F49" t="n">
         <v>1</v>
       </c>
       <c r="G49" t="n">
         <v>1</v>
+      </c>
+      <c r="H49" t="n">
+        <v>114</v>
       </c>
     </row>
     <row r="50">
@@ -1535,13 +1684,16 @@
         <v>0</v>
       </c>
       <c r="E50" t="n">
-        <v>6.981372833251953</v>
+        <v>31.32009506225586</v>
       </c>
       <c r="F50" t="n">
         <v>1</v>
       </c>
       <c r="G50" t="n">
         <v>1</v>
+      </c>
+      <c r="H50" t="n">
+        <v>168</v>
       </c>
     </row>
     <row r="51">
@@ -1560,12 +1712,15 @@
         <v>0</v>
       </c>
       <c r="E51" t="n">
-        <v>0</v>
+        <v>1.754045486450195</v>
       </c>
       <c r="F51" t="n">
         <v>0</v>
       </c>
       <c r="G51" t="n">
+        <v>0</v>
+      </c>
+      <c r="H51" t="n">
         <v>0</v>
       </c>
     </row>
@@ -1581,13 +1736,16 @@
         <v>0</v>
       </c>
       <c r="E52" t="n">
-        <v>2.987957000732422</v>
+        <v>2.371847629547119</v>
       </c>
       <c r="F52" t="n">
         <v>0</v>
       </c>
       <c r="G52" t="n">
         <v>0</v>
+      </c>
+      <c r="H52" t="n">
+        <v>29.99700029997</v>
       </c>
     </row>
     <row r="53">
@@ -1602,13 +1760,16 @@
         <v>0</v>
       </c>
       <c r="E53" t="n">
-        <v>3.989219665527344</v>
+        <v>2.705156803131104</v>
       </c>
       <c r="F53" t="n">
         <v>0</v>
       </c>
       <c r="G53" t="n">
         <v>0</v>
+      </c>
+      <c r="H53" t="n">
+        <v>60</v>
       </c>
     </row>
     <row r="54">
@@ -1617,19 +1778,22 @@
         <v>0.5</v>
       </c>
       <c r="C54" t="n">
-        <v>0.7169811320754716</v>
+        <v>0.2817460317460317</v>
       </c>
       <c r="D54" t="n">
         <v>0</v>
       </c>
       <c r="E54" t="n">
-        <v>4.986286163330078</v>
+        <v>3.317594528198242</v>
       </c>
       <c r="F54" t="n">
-        <v>0.625</v>
+        <v>0.1762749445676275</v>
       </c>
       <c r="G54" t="n">
-        <v>0.9629629629629629</v>
+        <v>0.936491935483871</v>
+      </c>
+      <c r="H54" t="n">
+        <v>72.0096012801707</v>
       </c>
     </row>
     <row r="55">
@@ -1638,19 +1802,22 @@
         <v>0.75</v>
       </c>
       <c r="C55" t="n">
-        <v>0.9898989898989899</v>
+        <v>0.9775193798449612</v>
       </c>
       <c r="D55" t="n">
         <v>0</v>
       </c>
       <c r="E55" t="n">
-        <v>5.983471870422363</v>
+        <v>3.917217254638672</v>
       </c>
       <c r="F55" t="n">
-        <v>1</v>
+        <v>0.9776515151515152</v>
       </c>
       <c r="G55" t="n">
         <v>1</v>
+      </c>
+      <c r="H55" t="n">
+        <v>85.88309518125703</v>
       </c>
     </row>
     <row r="56">
@@ -1665,13 +1832,16 @@
         <v>0</v>
       </c>
       <c r="E56" t="n">
-        <v>7.53355026245117</v>
+        <v>5.250608921051024</v>
       </c>
       <c r="F56" t="n">
         <v>1</v>
       </c>
       <c r="G56" t="n">
         <v>1</v>
+      </c>
+      <c r="H56" t="n">
+        <v>114</v>
       </c>
     </row>
     <row r="57">
@@ -1686,13 +1856,16 @@
         <v>0</v>
       </c>
       <c r="E57" t="n">
-        <v>51.86605453491211</v>
+        <v>24.80626106262207</v>
       </c>
       <c r="F57" t="n">
         <v>1</v>
       </c>
       <c r="G57" t="n">
         <v>1</v>
+      </c>
+      <c r="H57" t="n">
+        <v>168</v>
       </c>
     </row>
     <row r="58">
@@ -1711,12 +1884,15 @@
         <v>0</v>
       </c>
       <c r="E58" t="n">
-        <v>10.0092887878418</v>
+        <v>6.781816482543945</v>
       </c>
       <c r="F58" t="n">
         <v>0</v>
       </c>
       <c r="G58" t="n">
+        <v>0</v>
+      </c>
+      <c r="H58" t="n">
         <v>0</v>
       </c>
     </row>
@@ -1726,19 +1902,22 @@
         <v>0.05</v>
       </c>
       <c r="C59" t="n">
-        <v>0.3720930232558139</v>
+        <v>0.4444444444444444</v>
       </c>
       <c r="D59" t="n">
         <v>0</v>
       </c>
       <c r="E59" t="n">
-        <v>17.6771879196167</v>
+        <v>12.54597902297974</v>
       </c>
       <c r="F59" t="n">
-        <v>0.3694633408919123</v>
+        <v>0.3564849624060151</v>
       </c>
       <c r="G59" t="n">
-        <v>0.3085457271364318</v>
+        <v>0.6046428571428571</v>
+      </c>
+      <c r="H59" t="n">
+        <v>29.99700029997</v>
       </c>
     </row>
     <row r="60">
@@ -1747,19 +1926,22 @@
         <v>0.25</v>
       </c>
       <c r="C60" t="n">
-        <v>0.7580487804878049</v>
+        <v>0.8065930956423316</v>
       </c>
       <c r="D60" t="n">
         <v>0</v>
       </c>
       <c r="E60" t="n">
-        <v>24.69062805175781</v>
+        <v>18.54419708251953</v>
       </c>
       <c r="F60" t="n">
-        <v>0.8055555555555556</v>
+        <v>0.7272727272727273</v>
       </c>
       <c r="G60" t="n">
-        <v>0.7752525252525253</v>
+        <v>0.95</v>
+      </c>
+      <c r="H60" t="n">
+        <v>60</v>
       </c>
     </row>
     <row r="61">
@@ -1768,19 +1950,22 @@
         <v>0.5</v>
       </c>
       <c r="C61" t="n">
-        <v>0.9523809523809523</v>
+        <v>0.9459459459459459</v>
       </c>
       <c r="D61" t="n">
         <v>0</v>
       </c>
       <c r="E61" t="n">
-        <v>31.15105628967285</v>
+        <v>25.49302577972412</v>
       </c>
       <c r="F61" t="n">
-        <v>0.9583333333333334</v>
+        <v>0.925</v>
       </c>
       <c r="G61" t="n">
         <v>1</v>
+      </c>
+      <c r="H61" t="n">
+        <v>72.0096012801707</v>
       </c>
     </row>
     <row r="62">
@@ -1789,19 +1974,22 @@
         <v>0.75</v>
       </c>
       <c r="C62" t="n">
-        <v>0.9855072463768116</v>
+        <v>0.9836065573770492</v>
       </c>
       <c r="D62" t="n">
         <v>0</v>
       </c>
       <c r="E62" t="n">
-        <v>36.00382804870605</v>
+        <v>25.86674690246582</v>
       </c>
       <c r="F62" t="n">
-        <v>0.9722222222222222</v>
+        <v>0.9714285714285714</v>
       </c>
       <c r="G62" t="n">
         <v>1</v>
+      </c>
+      <c r="H62" t="n">
+        <v>85.88309518125703</v>
       </c>
     </row>
     <row r="63">
@@ -1810,19 +1998,22 @@
         <v>0.95</v>
       </c>
       <c r="C63" t="n">
-        <v>0.9882352941176471</v>
+        <v>0.9895496473141616</v>
       </c>
       <c r="D63" t="n">
         <v>0</v>
       </c>
       <c r="E63" t="n">
-        <v>50.72002410888671</v>
+        <v>26.46478414535522</v>
       </c>
       <c r="F63" t="n">
         <v>1</v>
       </c>
       <c r="G63" t="n">
         <v>1</v>
+      </c>
+      <c r="H63" t="n">
+        <v>114</v>
       </c>
     </row>
     <row r="64">
@@ -1837,13 +2028,16 @@
         <v>0</v>
       </c>
       <c r="E64" t="n">
-        <v>128.5982131958008</v>
+        <v>33.80465507507324</v>
       </c>
       <c r="F64" t="n">
         <v>1</v>
       </c>
       <c r="G64" t="n">
         <v>1</v>
+      </c>
+      <c r="H64" t="n">
+        <v>168</v>
       </c>
     </row>
     <row r="65">
@@ -1862,12 +2056,15 @@
         <v>0</v>
       </c>
       <c r="E65" t="n">
-        <v>0</v>
+        <v>2.09498405456543</v>
       </c>
       <c r="F65" t="n">
         <v>0</v>
       </c>
       <c r="G65" t="n">
+        <v>0</v>
+      </c>
+      <c r="H65" t="n">
         <v>0</v>
       </c>
     </row>
@@ -1877,19 +2074,22 @@
         <v>0.05</v>
       </c>
       <c r="C66" t="n">
-        <v>0.4232854864433812</v>
+        <v>0.7192820512820512</v>
       </c>
       <c r="D66" t="n">
         <v>0</v>
       </c>
       <c r="E66" t="n">
-        <v>1.560807228088379</v>
+        <v>2.288103103637695</v>
       </c>
       <c r="F66" t="n">
-        <v>0.6848214285714286</v>
+        <v>0.7676470588235295</v>
       </c>
       <c r="G66" t="n">
-        <v>0.2846153846153846</v>
+        <v>0.6930000000000001</v>
+      </c>
+      <c r="H66" t="n">
+        <v>29.99700029997</v>
       </c>
     </row>
     <row r="67">
@@ -1898,19 +2098,22 @@
         <v>0.25</v>
       </c>
       <c r="C67" t="n">
-        <v>0.8300000000000001</v>
+        <v>0.9591780821917808</v>
       </c>
       <c r="D67" t="n">
         <v>0</v>
       </c>
       <c r="E67" t="n">
-        <v>2.992987632751465</v>
+        <v>2.531230449676514</v>
       </c>
       <c r="F67" t="n">
-        <v>0.9672043010752689</v>
+        <v>0.9710144927536232</v>
       </c>
       <c r="G67" t="n">
-        <v>0.7936105476673427</v>
+        <v>0.9591836734693877</v>
+      </c>
+      <c r="H67" t="n">
+        <v>60</v>
       </c>
     </row>
     <row r="68">
@@ -1919,19 +2122,22 @@
         <v>0.5</v>
       </c>
       <c r="C68" t="n">
-        <v>0.9811320754716981</v>
+        <v>0.9866666666666667</v>
       </c>
       <c r="D68" t="n">
         <v>0</v>
       </c>
       <c r="E68" t="n">
-        <v>3.988981246948242</v>
+        <v>2.721071243286133</v>
       </c>
       <c r="F68" t="n">
         <v>1</v>
       </c>
       <c r="G68" t="n">
         <v>1</v>
+      </c>
+      <c r="H68" t="n">
+        <v>72.0096012801707</v>
       </c>
     </row>
     <row r="69">
@@ -1946,13 +2152,16 @@
         <v>0</v>
       </c>
       <c r="E69" t="n">
-        <v>4.962682723999023</v>
+        <v>2.892732620239258</v>
       </c>
       <c r="F69" t="n">
         <v>1</v>
       </c>
       <c r="G69" t="n">
         <v>1</v>
+      </c>
+      <c r="H69" t="n">
+        <v>85.88309518125703</v>
       </c>
     </row>
     <row r="70">
@@ -1967,13 +2176,16 @@
         <v>0</v>
       </c>
       <c r="E70" t="n">
-        <v>6.14309310913085</v>
+        <v>3.29867601394653</v>
       </c>
       <c r="F70" t="n">
         <v>1</v>
       </c>
       <c r="G70" t="n">
         <v>1</v>
+      </c>
+      <c r="H70" t="n">
+        <v>114</v>
       </c>
     </row>
     <row r="71">
@@ -1988,13 +2200,16 @@
         <v>0</v>
       </c>
       <c r="E71" t="n">
-        <v>25.92921257019043</v>
+        <v>7.384061813354492</v>
       </c>
       <c r="F71" t="n">
         <v>1</v>
       </c>
       <c r="G71" t="n">
         <v>1</v>
+      </c>
+      <c r="H71" t="n">
+        <v>168</v>
       </c>
     </row>
     <row r="72">
@@ -2013,12 +2228,15 @@
         <v>0</v>
       </c>
       <c r="E72" t="n">
-        <v>0</v>
+        <v>1.234292984008789</v>
       </c>
       <c r="F72" t="n">
         <v>0</v>
       </c>
       <c r="G72" t="n">
+        <v>0</v>
+      </c>
+      <c r="H72" t="n">
         <v>0</v>
       </c>
     </row>
@@ -2034,13 +2252,16 @@
         <v>0</v>
       </c>
       <c r="E73" t="n">
-        <v>1.089262962341309</v>
+        <v>1.362955570220947</v>
       </c>
       <c r="F73" t="n">
         <v>0</v>
       </c>
       <c r="G73" t="n">
         <v>0</v>
+      </c>
+      <c r="H73" t="n">
+        <v>29.99700029997</v>
       </c>
     </row>
     <row r="74">
@@ -2049,19 +2270,22 @@
         <v>0.25</v>
       </c>
       <c r="C74" t="n">
-        <v>0.2910628019323672</v>
+        <v>0.6715292903817494</v>
       </c>
       <c r="D74" t="n">
         <v>0</v>
       </c>
       <c r="E74" t="n">
-        <v>1.99580192565918</v>
+        <v>1.804351806640625</v>
       </c>
       <c r="F74" t="n">
-        <v>0.3660714285714286</v>
+        <v>0.9781249999999999</v>
       </c>
       <c r="G74" t="n">
-        <v>0.205010775862069</v>
+        <v>0.5258859784283514</v>
+      </c>
+      <c r="H74" t="n">
+        <v>60</v>
       </c>
     </row>
     <row r="75">
@@ -2070,19 +2294,22 @@
         <v>0.5</v>
       </c>
       <c r="C75" t="n">
-        <v>0.9583333333333334</v>
+        <v>0.9508196721311475</v>
       </c>
       <c r="D75" t="n">
         <v>0</v>
       </c>
       <c r="E75" t="n">
-        <v>2.991676330566406</v>
+        <v>2.243518829345703</v>
       </c>
       <c r="F75" t="n">
         <v>1</v>
       </c>
       <c r="G75" t="n">
-        <v>0.9399999999999999</v>
+        <v>0.911437908496732</v>
+      </c>
+      <c r="H75" t="n">
+        <v>72.0096012801707</v>
       </c>
     </row>
     <row r="76">
@@ -2091,19 +2318,22 @@
         <v>0.75</v>
       </c>
       <c r="C76" t="n">
-        <v>0.987878342638848</v>
+        <v>0.9859154929577465</v>
       </c>
       <c r="D76" t="n">
         <v>0</v>
       </c>
       <c r="E76" t="n">
-        <v>3.46672534942627</v>
+        <v>2.484798431396484</v>
       </c>
       <c r="F76" t="n">
         <v>1</v>
       </c>
       <c r="G76" t="n">
-        <v>1</v>
+        <v>0.9849598163030999</v>
+      </c>
+      <c r="H76" t="n">
+        <v>85.88309518125703</v>
       </c>
     </row>
     <row r="77">
@@ -2118,13 +2348,16 @@
         <v>0</v>
       </c>
       <c r="E77" t="n">
-        <v>4.960036277770994</v>
+        <v>2.801764011383057</v>
       </c>
       <c r="F77" t="n">
         <v>1</v>
       </c>
       <c r="G77" t="n">
         <v>1</v>
+      </c>
+      <c r="H77" t="n">
+        <v>114</v>
       </c>
     </row>
     <row r="78">
@@ -2139,13 +2372,16 @@
         <v>0</v>
       </c>
       <c r="E78" t="n">
-        <v>7.542610168457031</v>
+        <v>4.097223281860352</v>
       </c>
       <c r="F78" t="n">
         <v>1</v>
       </c>
       <c r="G78" t="n">
         <v>1</v>
+      </c>
+      <c r="H78" t="n">
+        <v>168</v>
       </c>
     </row>
     <row r="79">
@@ -2172,6 +2408,9 @@
       <c r="G79" t="n">
         <v>0</v>
       </c>
+      <c r="H79" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="80">
       <c r="A80" s="1" t="n"/>
@@ -2179,19 +2418,22 @@
         <v>0.05</v>
       </c>
       <c r="C80" t="n">
-        <v>0</v>
+        <v>0.2339285714285717</v>
       </c>
       <c r="D80" t="n">
         <v>0</v>
       </c>
       <c r="E80" t="n">
-        <v>8.764576911926273</v>
+        <v>1.7992999994196</v>
       </c>
       <c r="F80" t="n">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="G80" t="n">
-        <v>0</v>
+        <v>0.1536111111111111</v>
+      </c>
+      <c r="H80" t="n">
+        <v>29.99700029997</v>
       </c>
     </row>
     <row r="81">
@@ -2200,19 +2442,22 @@
         <v>0.25</v>
       </c>
       <c r="C81" t="n">
-        <v>0.8333333333333334</v>
+        <v>0.925</v>
       </c>
       <c r="D81" t="n">
         <v>0</v>
       </c>
       <c r="E81" t="n">
-        <v>13.40866088867188</v>
+        <v>2.188000001013279</v>
       </c>
       <c r="F81" t="n">
-        <v>0.9642857142857143</v>
+        <v>0.9565217391304348</v>
       </c>
       <c r="G81" t="n">
-        <v>0.7575757575757576</v>
+        <v>0.9115942028985506</v>
+      </c>
+      <c r="H81" t="n">
+        <v>60</v>
       </c>
     </row>
     <row r="82">
@@ -2221,19 +2466,22 @@
         <v>0.5</v>
       </c>
       <c r="C82" t="n">
-        <v>0.9824561403508771</v>
+        <v>0.9803921568627451</v>
       </c>
       <c r="D82" t="n">
         <v>0</v>
       </c>
       <c r="E82" t="n">
-        <v>16.92461967468262</v>
+        <v>2.438499998301268</v>
       </c>
       <c r="F82" t="n">
         <v>1</v>
       </c>
       <c r="G82" t="n">
-        <v>1</v>
+        <v>0.975</v>
+      </c>
+      <c r="H82" t="n">
+        <v>72.0096012801707</v>
       </c>
     </row>
     <row r="83">
@@ -2248,13 +2496,16 @@
         <v>0</v>
       </c>
       <c r="E83" t="n">
-        <v>19.94979381561279</v>
+        <v>2.983499999158084</v>
       </c>
       <c r="F83" t="n">
         <v>1</v>
       </c>
       <c r="G83" t="n">
         <v>1</v>
+      </c>
+      <c r="H83" t="n">
+        <v>85.88309518125703</v>
       </c>
     </row>
     <row r="84">
@@ -2269,13 +2520,16 @@
         <v>0</v>
       </c>
       <c r="E84" t="n">
-        <v>28.31723690032959</v>
+        <v>6.400450000446289</v>
       </c>
       <c r="F84" t="n">
         <v>1</v>
       </c>
       <c r="G84" t="n">
         <v>1</v>
+      </c>
+      <c r="H84" t="n">
+        <v>114</v>
       </c>
     </row>
     <row r="85">
@@ -2290,13 +2544,16 @@
         <v>1</v>
       </c>
       <c r="E85" t="n">
-        <v>662.0008945465088</v>
+        <v>27.7690000012517</v>
       </c>
       <c r="F85" t="n">
         <v>1</v>
       </c>
       <c r="G85" t="n">
         <v>1</v>
+      </c>
+      <c r="H85" t="n">
+        <v>168</v>
       </c>
     </row>
     <row r="86">
@@ -2323,6 +2580,9 @@
       <c r="G86" t="n">
         <v>0</v>
       </c>
+      <c r="H86" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="87">
       <c r="A87" s="1" t="n"/>
@@ -2336,13 +2596,16 @@
         <v>0</v>
       </c>
       <c r="E87" t="n">
-        <v>15.50219058990479</v>
+        <v>0.6260000001231674</v>
       </c>
       <c r="F87" t="n">
         <v>0</v>
       </c>
       <c r="G87" t="n">
         <v>0</v>
+      </c>
+      <c r="H87" t="n">
+        <v>29.99700029997</v>
       </c>
     </row>
     <row r="88">
@@ -2351,19 +2614,22 @@
         <v>0.25</v>
       </c>
       <c r="C88" t="n">
-        <v>0.3601962741184298</v>
+        <v>0.2673208682845617</v>
       </c>
       <c r="D88" t="n">
         <v>0</v>
       </c>
       <c r="E88" t="n">
-        <v>18.66769790649414</v>
+        <v>0.8672500043176115</v>
       </c>
       <c r="F88" t="n">
-        <v>0.90935192780968</v>
+        <v>0.945933014354067</v>
       </c>
       <c r="G88" t="n">
-        <v>0.2734572837531654</v>
+        <v>0.1716376898481215</v>
+      </c>
+      <c r="H88" t="n">
+        <v>60</v>
       </c>
     </row>
     <row r="89">
@@ -2372,19 +2638,22 @@
         <v>0.5</v>
       </c>
       <c r="C89" t="n">
-        <v>0.8787878787878788</v>
+        <v>0.6063089915548932</v>
       </c>
       <c r="D89" t="n">
         <v>0</v>
       </c>
       <c r="E89" t="n">
-        <v>21.09289169311523</v>
+        <v>1.040000000037253</v>
       </c>
       <c r="F89" t="n">
         <v>1</v>
       </c>
       <c r="G89" t="n">
-        <v>0.8333333333333334</v>
+        <v>0.521286231884058</v>
+      </c>
+      <c r="H89" t="n">
+        <v>72.0096012801707</v>
       </c>
     </row>
     <row r="90">
@@ -2393,19 +2662,22 @@
         <v>0.75</v>
       </c>
       <c r="C90" t="n">
-        <v>1</v>
+        <v>0.9844932844932845</v>
       </c>
       <c r="D90" t="n">
         <v>0</v>
       </c>
       <c r="E90" t="n">
-        <v>23.22590351104736</v>
+        <v>1.471000000834465</v>
       </c>
       <c r="F90" t="n">
         <v>1</v>
       </c>
       <c r="G90" t="n">
-        <v>1</v>
+        <v>0.9772727272727273</v>
+      </c>
+      <c r="H90" t="n">
+        <v>85.88309518125703</v>
       </c>
     </row>
     <row r="91">
@@ -2420,13 +2692,16 @@
         <v>0</v>
       </c>
       <c r="E91" t="n">
-        <v>27.9299259185791</v>
+        <v>1.97135000154376</v>
       </c>
       <c r="F91" t="n">
         <v>1</v>
       </c>
       <c r="G91" t="n">
         <v>1</v>
+      </c>
+      <c r="H91" t="n">
+        <v>114</v>
       </c>
     </row>
     <row r="92">
@@ -2441,13 +2716,16 @@
         <v>1</v>
       </c>
       <c r="E92" t="n">
-        <v>172.8610992431641</v>
+        <v>17.2390000000596</v>
       </c>
       <c r="F92" t="n">
         <v>1</v>
       </c>
       <c r="G92" t="n">
         <v>1</v>
+      </c>
+      <c r="H92" t="n">
+        <v>168</v>
       </c>
     </row>
     <row r="93">
@@ -2466,12 +2744,15 @@
         <v>0</v>
       </c>
       <c r="E93" t="n">
-        <v>0</v>
+        <v>2.932071685791016</v>
       </c>
       <c r="F93" t="n">
         <v>0</v>
       </c>
       <c r="G93" t="n">
+        <v>0</v>
+      </c>
+      <c r="H93" t="n">
         <v>0</v>
       </c>
     </row>
@@ -2481,19 +2762,22 @@
         <v>0.05</v>
       </c>
       <c r="C94" t="n">
-        <v>0.3621428571428572</v>
+        <v>0.7172395557905871</v>
       </c>
       <c r="D94" t="n">
         <v>0</v>
       </c>
       <c r="E94" t="n">
-        <v>3.989696502685547</v>
+        <v>5.411064624786377</v>
       </c>
       <c r="F94" t="n">
-        <v>0.9135416666666667</v>
+        <v>0.9230769230769231</v>
       </c>
       <c r="G94" t="n">
-        <v>0.2264033264033264</v>
+        <v>0.5618357487922706</v>
+      </c>
+      <c r="H94" t="n">
+        <v>29.99700029997</v>
       </c>
     </row>
     <row r="95">
@@ -2502,19 +2786,22 @@
         <v>0.25</v>
       </c>
       <c r="C95" t="n">
-        <v>0.8207949696833595</v>
+        <v>0.9428571428571428</v>
       </c>
       <c r="D95" t="n">
         <v>0</v>
       </c>
       <c r="E95" t="n">
-        <v>6.02412223815918</v>
+        <v>6.798803806304932</v>
       </c>
       <c r="F95" t="n">
-        <v>0.9789450354609929</v>
+        <v>0.9757549361207898</v>
       </c>
       <c r="G95" t="n">
-        <v>0.717670011148272</v>
+        <v>0.9090909090909091</v>
+      </c>
+      <c r="H95" t="n">
+        <v>60</v>
       </c>
     </row>
     <row r="96">
@@ -2523,19 +2810,22 @@
         <v>0.5</v>
       </c>
       <c r="C96" t="n">
-        <v>0.9818181818181818</v>
+        <v>0.9855072463768116</v>
       </c>
       <c r="D96" t="n">
         <v>0</v>
       </c>
       <c r="E96" t="n">
-        <v>8.018255233764648</v>
+        <v>9.033441543579102</v>
       </c>
       <c r="F96" t="n">
         <v>1</v>
       </c>
       <c r="G96" t="n">
         <v>1</v>
+      </c>
+      <c r="H96" t="n">
+        <v>72.0096012801707</v>
       </c>
     </row>
     <row r="97">
@@ -2550,13 +2840,16 @@
         <v>0</v>
       </c>
       <c r="E97" t="n">
-        <v>10.10191440582275</v>
+        <v>9.128272533416748</v>
       </c>
       <c r="F97" t="n">
         <v>1</v>
       </c>
       <c r="G97" t="n">
         <v>1</v>
+      </c>
+      <c r="H97" t="n">
+        <v>85.88309518125703</v>
       </c>
     </row>
     <row r="98">
@@ -2571,13 +2864,16 @@
         <v>0</v>
       </c>
       <c r="E98" t="n">
-        <v>13.97163867950439</v>
+        <v>9.864449501037598</v>
       </c>
       <c r="F98" t="n">
         <v>1</v>
       </c>
       <c r="G98" t="n">
         <v>1</v>
+      </c>
+      <c r="H98" t="n">
+        <v>114</v>
       </c>
     </row>
     <row r="99">
@@ -2592,13 +2888,16 @@
         <v>0</v>
       </c>
       <c r="E99" t="n">
-        <v>40.64726829528809</v>
+        <v>11.87396049499512</v>
       </c>
       <c r="F99" t="n">
         <v>1</v>
       </c>
       <c r="G99" t="n">
         <v>1</v>
+      </c>
+      <c r="H99" t="n">
+        <v>168</v>
       </c>
     </row>
     <row r="100">
@@ -2617,12 +2916,15 @@
         <v>0</v>
       </c>
       <c r="E100" t="n">
-        <v>23.79775047302246</v>
+        <v>8.366999998688698</v>
       </c>
       <c r="F100" t="n">
         <v>0</v>
       </c>
       <c r="G100" t="n">
+        <v>0</v>
+      </c>
+      <c r="H100" t="n">
         <v>0</v>
       </c>
     </row>
@@ -2632,19 +2934,22 @@
         <v>0.05</v>
       </c>
       <c r="C101" t="n">
-        <v>0.4130150173276858</v>
+        <v>0.6958314034275129</v>
       </c>
       <c r="D101" t="n">
         <v>0</v>
       </c>
       <c r="E101" t="n">
-        <v>29.59902286529541</v>
+        <v>12.15984999995562</v>
       </c>
       <c r="F101" t="n">
-        <v>0.9143939393939394</v>
+        <v>0.8991025641025642</v>
       </c>
       <c r="G101" t="n">
-        <v>0.2647279549718575</v>
+        <v>0.5731907894736843</v>
+      </c>
+      <c r="H101" t="n">
+        <v>29.99700029997</v>
       </c>
     </row>
     <row r="102">
@@ -2653,19 +2958,22 @@
         <v>0.25</v>
       </c>
       <c r="C102" t="n">
-        <v>0.8452991452991453</v>
+        <v>0.9696969696969697</v>
       </c>
       <c r="D102" t="n">
         <v>0</v>
       </c>
       <c r="E102" t="n">
-        <v>32.86218643188477</v>
+        <v>18.17775000073016</v>
       </c>
       <c r="F102" t="n">
         <v>1</v>
       </c>
       <c r="G102" t="n">
-        <v>0.7464285714285714</v>
+        <v>0.9523809523809523</v>
+      </c>
+      <c r="H102" t="n">
+        <v>60</v>
       </c>
     </row>
     <row r="103">
@@ -2674,19 +2982,22 @@
         <v>0.5</v>
       </c>
       <c r="C103" t="n">
-        <v>0.9859154929577465</v>
+        <v>0.9873417721518988</v>
       </c>
       <c r="D103" t="n">
         <v>0</v>
       </c>
       <c r="E103" t="n">
-        <v>40.01116752624512</v>
+        <v>36.82699999865144</v>
       </c>
       <c r="F103" t="n">
         <v>1</v>
       </c>
       <c r="G103" t="n">
-        <v>1</v>
+        <v>0.9782608695652174</v>
+      </c>
+      <c r="H103" t="n">
+        <v>72.0096012801707</v>
       </c>
     </row>
     <row r="104">
@@ -2701,13 +3012,16 @@
         <v>0</v>
       </c>
       <c r="E104" t="n">
-        <v>53.99167537689209</v>
+        <v>39.12900000018999</v>
       </c>
       <c r="F104" t="n">
         <v>1</v>
       </c>
       <c r="G104" t="n">
         <v>1</v>
+      </c>
+      <c r="H104" t="n">
+        <v>85.88309518125703</v>
       </c>
     </row>
     <row r="105">
@@ -2722,13 +3036,16 @@
         <v>0</v>
       </c>
       <c r="E105" t="n">
-        <v>80.77621459960935</v>
+        <v>45.38795000091195</v>
       </c>
       <c r="F105" t="n">
         <v>1</v>
       </c>
       <c r="G105" t="n">
         <v>1</v>
+      </c>
+      <c r="H105" t="n">
+        <v>114</v>
       </c>
     </row>
     <row r="106">
@@ -2743,13 +3060,16 @@
         <v>0</v>
       </c>
       <c r="E106" t="n">
-        <v>393.5410976409912</v>
+        <v>75.85600000061095</v>
       </c>
       <c r="F106" t="n">
         <v>1</v>
       </c>
       <c r="G106" t="n">
         <v>1</v>
+      </c>
+      <c r="H106" t="n">
+        <v>168</v>
       </c>
     </row>
     <row r="107">
@@ -2768,12 +3088,15 @@
         <v>0</v>
       </c>
       <c r="E107" t="n">
-        <v>88.8063907623291</v>
+        <v>63.14706802368164</v>
       </c>
       <c r="F107" t="n">
         <v>0</v>
       </c>
       <c r="G107" t="n">
+        <v>0</v>
+      </c>
+      <c r="H107" t="n">
         <v>0</v>
       </c>
     </row>
@@ -2783,19 +3106,22 @@
         <v>0.05</v>
       </c>
       <c r="C108" t="n">
-        <v>0.2823529411764706</v>
+        <v>0.4259398496240602</v>
       </c>
       <c r="D108" t="n">
         <v>0</v>
       </c>
       <c r="E108" t="n">
-        <v>169.935941696167</v>
+        <v>126.787805557251</v>
       </c>
       <c r="F108" t="n">
-        <v>0.6207407407407408</v>
+        <v>0.6</v>
       </c>
       <c r="G108" t="n">
-        <v>0.1953194180898166</v>
+        <v>0.3846153846153846</v>
+      </c>
+      <c r="H108" t="n">
+        <v>29.99700029997</v>
       </c>
     </row>
     <row r="109">
@@ -2804,19 +3130,22 @@
         <v>0.25</v>
       </c>
       <c r="C109" t="n">
-        <v>0.7097222222222223</v>
+        <v>0.7567567567567568</v>
       </c>
       <c r="D109" t="n">
         <v>0</v>
       </c>
       <c r="E109" t="n">
-        <v>243.1625127792358</v>
+        <v>185.9567761421204</v>
       </c>
       <c r="F109" t="n">
-        <v>0.9652147610405324</v>
+        <v>0.8521241830065359</v>
       </c>
       <c r="G109" t="n">
-        <v>0.5816666666666667</v>
+        <v>0.6818181818181818</v>
+      </c>
+      <c r="H109" t="n">
+        <v>60</v>
       </c>
     </row>
     <row r="110">
@@ -2825,19 +3154,22 @@
         <v>0.5</v>
       </c>
       <c r="C110" t="n">
-        <v>0.8732394366197183</v>
+        <v>0.8979933110367893</v>
       </c>
       <c r="D110" t="n">
         <v>0</v>
       </c>
       <c r="E110" t="n">
-        <v>280.7493209838867</v>
+        <v>258.938193321228</v>
       </c>
       <c r="F110" t="n">
         <v>1</v>
       </c>
       <c r="G110" t="n">
-        <v>0.8108108108108109</v>
+        <v>0.9028324154209284</v>
+      </c>
+      <c r="H110" t="n">
+        <v>72.0096012801707</v>
       </c>
     </row>
     <row r="111">
@@ -2846,19 +3178,22 @@
         <v>0.75</v>
       </c>
       <c r="C111" t="n">
-        <v>0.9855072463768116</v>
+        <v>0.9761904761904762</v>
       </c>
       <c r="D111" t="n">
         <v>0</v>
       </c>
       <c r="E111" t="n">
-        <v>357.7612638473511</v>
+        <v>261.0234618186951</v>
       </c>
       <c r="F111" t="n">
         <v>1</v>
       </c>
       <c r="G111" t="n">
-        <v>0.9722222222222222</v>
+        <v>0.9736842105263158</v>
+      </c>
+      <c r="H111" t="n">
+        <v>85.88309518125703</v>
       </c>
     </row>
     <row r="112">
@@ -2867,19 +3202,22 @@
         <v>0.95</v>
       </c>
       <c r="C112" t="n">
-        <v>0.9911504424778761</v>
+        <v>0.9923686477174849</v>
       </c>
       <c r="D112" t="n">
         <v>0</v>
       </c>
       <c r="E112" t="n">
-        <v>451.9218683242794</v>
+        <v>265.5675768852234</v>
       </c>
       <c r="F112" t="n">
         <v>1</v>
       </c>
       <c r="G112" t="n">
         <v>1</v>
+      </c>
+      <c r="H112" t="n">
+        <v>114</v>
       </c>
     </row>
     <row r="113">
@@ -2894,13 +3232,16 @@
         <v>0</v>
       </c>
       <c r="E113" t="n">
-        <v>620.9404468536377</v>
+        <v>382.7800750732422</v>
       </c>
       <c r="F113" t="n">
         <v>1</v>
       </c>
       <c r="G113" t="n">
         <v>1</v>
+      </c>
+      <c r="H113" t="n">
+        <v>168</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Generated results on 6th Jan 2023
Includes two new algorithms, and ran fine (after re-running analysis on all datasets)
</commit_message>
<xml_diff>
--- a/Algorithm_tester/data_autosave/real_overall.xlsx
+++ b/Algorithm_tester/data_autosave/real_overall.xlsx
@@ -446,7 +446,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H113"/>
+  <dimension ref="A1:H127"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -508,7 +508,7 @@
         <v>0</v>
       </c>
       <c r="E2" t="n">
-        <v>60.35780906677246</v>
+        <v>61.4469051361084</v>
       </c>
       <c r="F2" t="n">
         <v>0</v>
@@ -532,7 +532,7 @@
         <v>0</v>
       </c>
       <c r="E3" t="n">
-        <v>111.6964221000671</v>
+        <v>114.3857836723328</v>
       </c>
       <c r="F3" t="n">
         <v>0.04516885553470926</v>
@@ -556,7 +556,7 @@
         <v>0</v>
       </c>
       <c r="E4" t="n">
-        <v>156.716525554657</v>
+        <v>158.9834690093994</v>
       </c>
       <c r="F4" t="n">
         <v>0.9736842105263158</v>
@@ -580,7 +580,7 @@
         <v>0</v>
       </c>
       <c r="E5" t="n">
-        <v>197.9329586029053</v>
+        <v>197.0813274383545</v>
       </c>
       <c r="F5" t="n">
         <v>1</v>
@@ -604,7 +604,7 @@
         <v>0</v>
       </c>
       <c r="E6" t="n">
-        <v>211.6356492042542</v>
+        <v>210.39217710495</v>
       </c>
       <c r="F6" t="n">
         <v>1</v>
@@ -628,7 +628,7 @@
         <v>0</v>
       </c>
       <c r="E7" t="n">
-        <v>230.163586139679</v>
+        <v>229.6232342720032</v>
       </c>
       <c r="F7" t="n">
         <v>1</v>
@@ -652,7 +652,7 @@
         <v>0</v>
       </c>
       <c r="E8" t="n">
-        <v>252.3441314697266</v>
+        <v>947360.002040863</v>
       </c>
       <c r="F8" t="n">
         <v>1</v>
@@ -728,7 +728,7 @@
         <v>0</v>
       </c>
       <c r="E11" t="n">
-        <v>47.7641224861145</v>
+        <v>47.71411418914795</v>
       </c>
       <c r="F11" t="n">
         <v>0.08522727272727272</v>
@@ -752,7 +752,7 @@
         <v>0</v>
       </c>
       <c r="E12" t="n">
-        <v>67.58248805999756</v>
+        <v>67.60001182556152</v>
       </c>
       <c r="F12" t="n">
         <v>0.5384615384615384</v>
@@ -776,7 +776,7 @@
         <v>0</v>
       </c>
       <c r="E13" t="n">
-        <v>84.20681953430176</v>
+        <v>84.39451456069946</v>
       </c>
       <c r="F13" t="n">
         <v>0.9266034327009938</v>
@@ -800,7 +800,7 @@
         <v>1</v>
       </c>
       <c r="E14" t="n">
-        <v>93.55617761611938</v>
+        <v>95.12854814529419</v>
       </c>
       <c r="F14" t="n">
         <v>0.9772727272727273</v>
@@ -824,7 +824,7 @@
         <v>1</v>
       </c>
       <c r="E15" t="n">
-        <v>156.6369533538818</v>
+        <v>1027272.235155106</v>
       </c>
       <c r="F15" t="n">
         <v>1</v>
@@ -839,7 +839,7 @@
     <row r="16">
       <c r="A16" s="1" t="inlineStr">
         <is>
-          <t>gamb</t>
+          <t>fnvg</t>
         </is>
       </c>
       <c r="B16" s="1" t="n">
@@ -852,7 +852,7 @@
         <v>0</v>
       </c>
       <c r="E16" t="n">
-        <v>0</v>
+        <v>10.55812835693359</v>
       </c>
       <c r="F16" t="n">
         <v>0</v>
@@ -876,7 +876,7 @@
         <v>0</v>
       </c>
       <c r="E17" t="n">
-        <v>0</v>
+        <v>14.80237245559692</v>
       </c>
       <c r="F17" t="n">
         <v>0</v>
@@ -894,19 +894,19 @@
         <v>0.25</v>
       </c>
       <c r="C18" t="n">
-        <v>0</v>
+        <v>0.8980769230769231</v>
       </c>
       <c r="D18" t="n">
         <v>0</v>
       </c>
       <c r="E18" t="n">
-        <v>0</v>
+        <v>18.50450038909912</v>
       </c>
       <c r="F18" t="n">
-        <v>0</v>
+        <v>0.9773989898989899</v>
       </c>
       <c r="G18" t="n">
-        <v>0</v>
+        <v>0.8796791443850267</v>
       </c>
       <c r="H18" t="n">
         <v>60</v>
@@ -918,19 +918,19 @@
         <v>0.5</v>
       </c>
       <c r="C19" t="n">
-        <v>0.4196009389671361</v>
+        <v>0.9791666666666666</v>
       </c>
       <c r="D19" t="n">
         <v>0</v>
       </c>
       <c r="E19" t="n">
-        <v>1.990437507629395</v>
+        <v>22.92704582214355</v>
       </c>
       <c r="F19" t="n">
-        <v>0.9074074074074074</v>
+        <v>1</v>
       </c>
       <c r="G19" t="n">
-        <v>0.2655075187969925</v>
+        <v>0.9722222222222222</v>
       </c>
       <c r="H19" t="n">
         <v>72.0096012801707</v>
@@ -942,19 +942,19 @@
         <v>0.75</v>
       </c>
       <c r="C20" t="n">
-        <v>0.6322537112010795</v>
+        <v>1</v>
       </c>
       <c r="D20" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E20" t="n">
-        <v>2.715766429901123</v>
+        <v>23.75596761703491</v>
       </c>
       <c r="F20" t="n">
         <v>1</v>
       </c>
       <c r="G20" t="n">
-        <v>0.4625</v>
+        <v>1</v>
       </c>
       <c r="H20" t="n">
         <v>85.88309518125703</v>
@@ -966,19 +966,19 @@
         <v>0.95</v>
       </c>
       <c r="C21" t="n">
-        <v>0.8343939393939391</v>
+        <v>1</v>
       </c>
       <c r="D21" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E21" t="n">
-        <v>5.116319656372069</v>
+        <v>25.59356689453125</v>
       </c>
       <c r="F21" t="n">
         <v>1</v>
       </c>
       <c r="G21" t="n">
-        <v>0.7231944444444441</v>
+        <v>1</v>
       </c>
       <c r="H21" t="n">
         <v>114</v>
@@ -993,10 +993,10 @@
         <v>1</v>
       </c>
       <c r="D22" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E22" t="n">
-        <v>78.72581481933594</v>
+        <v>45.31693458557129</v>
       </c>
       <c r="F22" t="n">
         <v>1</v>
@@ -1011,7 +1011,7 @@
     <row r="23">
       <c r="A23" s="1" t="inlineStr">
         <is>
-          <t>gqrs</t>
+          <t>fwhvg</t>
         </is>
       </c>
       <c r="B23" s="1" t="n">
@@ -1024,7 +1024,7 @@
         <v>0</v>
       </c>
       <c r="E23" t="n">
-        <v>0</v>
+        <v>10.35380363464355</v>
       </c>
       <c r="F23" t="n">
         <v>0</v>
@@ -1042,19 +1042,19 @@
         <v>0.05</v>
       </c>
       <c r="C24" t="n">
-        <v>0.4722442244224423</v>
+        <v>0</v>
       </c>
       <c r="D24" t="n">
         <v>0</v>
       </c>
       <c r="E24" t="n">
-        <v>62.21141815185547</v>
+        <v>14.6068811416626</v>
       </c>
       <c r="F24" t="n">
-        <v>0.7145909090909092</v>
+        <v>0</v>
       </c>
       <c r="G24" t="n">
-        <v>0.3182739726027398</v>
+        <v>0</v>
       </c>
       <c r="H24" t="n">
         <v>29.99700029997</v>
@@ -1066,19 +1066,19 @@
         <v>0.25</v>
       </c>
       <c r="C25" t="n">
-        <v>0.6666666666666666</v>
+        <v>0.8980769230769231</v>
       </c>
       <c r="D25" t="n">
         <v>0</v>
       </c>
       <c r="E25" t="n">
-        <v>88.17487955093384</v>
+        <v>18.28336715698242</v>
       </c>
       <c r="F25" t="n">
-        <v>0.972972972972973</v>
+        <v>0.9773989898989899</v>
       </c>
       <c r="G25" t="n">
-        <v>0.5068493150684932</v>
+        <v>0.8796791443850267</v>
       </c>
       <c r="H25" t="n">
         <v>60</v>
@@ -1090,19 +1090,19 @@
         <v>0.5</v>
       </c>
       <c r="C26" t="n">
-        <v>0.8489256639530228</v>
+        <v>0.9791666666666666</v>
       </c>
       <c r="D26" t="n">
         <v>0</v>
       </c>
       <c r="E26" t="n">
-        <v>121.5285062789917</v>
+        <v>22.47047424316406</v>
       </c>
       <c r="F26" t="n">
         <v>1</v>
       </c>
       <c r="G26" t="n">
-        <v>0.8636363636363636</v>
+        <v>0.9722222222222222</v>
       </c>
       <c r="H26" t="n">
         <v>72.0096012801707</v>
@@ -1114,13 +1114,13 @@
         <v>0.75</v>
       </c>
       <c r="C27" t="n">
-        <v>0.9906542056074766</v>
+        <v>1</v>
       </c>
       <c r="D27" t="n">
         <v>0</v>
       </c>
       <c r="E27" t="n">
-        <v>133.4934234619141</v>
+        <v>23.33343029022217</v>
       </c>
       <c r="F27" t="n">
         <v>1</v>
@@ -1144,7 +1144,7 @@
         <v>0</v>
       </c>
       <c r="E28" t="n">
-        <v>142.6933765411377</v>
+        <v>25.12226104736328</v>
       </c>
       <c r="F28" t="n">
         <v>1</v>
@@ -1165,10 +1165,10 @@
         <v>1</v>
       </c>
       <c r="D29" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E29" t="n">
-        <v>156.9509506225586</v>
+        <v>954233.4611415863</v>
       </c>
       <c r="F29" t="n">
         <v>1</v>
@@ -1183,7 +1183,7 @@
     <row r="30">
       <c r="A30" s="1" t="inlineStr">
         <is>
-          <t>hamilt</t>
+          <t>gamb</t>
         </is>
       </c>
       <c r="B30" s="1" t="n">
@@ -1196,7 +1196,7 @@
         <v>0</v>
       </c>
       <c r="E30" t="n">
-        <v>-36.56482696533203</v>
+        <v>0</v>
       </c>
       <c r="F30" t="n">
         <v>0</v>
@@ -1220,7 +1220,7 @@
         <v>0</v>
       </c>
       <c r="E31" t="n">
-        <v>8.170735836029053</v>
+        <v>0</v>
       </c>
       <c r="F31" t="n">
         <v>0</v>
@@ -1238,19 +1238,19 @@
         <v>0.25</v>
       </c>
       <c r="C32" t="n">
-        <v>0.7444140446876425</v>
+        <v>0</v>
       </c>
       <c r="D32" t="n">
         <v>0</v>
       </c>
       <c r="E32" t="n">
-        <v>11.03270053863525</v>
+        <v>0</v>
       </c>
       <c r="F32" t="n">
-        <v>0.976328903654485</v>
+        <v>0</v>
       </c>
       <c r="G32" t="n">
-        <v>0.6205555555555555</v>
+        <v>0</v>
       </c>
       <c r="H32" t="n">
         <v>60</v>
@@ -1262,19 +1262,19 @@
         <v>0.5</v>
       </c>
       <c r="C33" t="n">
-        <v>0.9536672629695886</v>
+        <v>0.4196009389671361</v>
       </c>
       <c r="D33" t="n">
         <v>0</v>
       </c>
       <c r="E33" t="n">
-        <v>16.98446273803711</v>
+        <v>1.989006996154785</v>
       </c>
       <c r="F33" t="n">
-        <v>1</v>
+        <v>0.9074074074074074</v>
       </c>
       <c r="G33" t="n">
-        <v>0.9230769230769231</v>
+        <v>0.2655075187969925</v>
       </c>
       <c r="H33" t="n">
         <v>72.0096012801707</v>
@@ -1286,19 +1286,19 @@
         <v>0.75</v>
       </c>
       <c r="C34" t="n">
-        <v>0.9855072463768116</v>
+        <v>0.6322537112010795</v>
       </c>
       <c r="D34" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E34" t="n">
-        <v>19.25581693649292</v>
+        <v>2.639949321746826</v>
       </c>
       <c r="F34" t="n">
         <v>1</v>
       </c>
       <c r="G34" t="n">
-        <v>0.9741902834008097</v>
+        <v>0.4625</v>
       </c>
       <c r="H34" t="n">
         <v>85.88309518125703</v>
@@ -1310,19 +1310,19 @@
         <v>0.95</v>
       </c>
       <c r="C35" t="n">
-        <v>1</v>
+        <v>0.8343939393939391</v>
       </c>
       <c r="D35" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E35" t="n">
-        <v>21.28853797912598</v>
+        <v>8.520698547363253</v>
       </c>
       <c r="F35" t="n">
         <v>1</v>
       </c>
       <c r="G35" t="n">
-        <v>1</v>
+        <v>0.7231944444444441</v>
       </c>
       <c r="H35" t="n">
         <v>114</v>
@@ -1337,10 +1337,10 @@
         <v>1</v>
       </c>
       <c r="D36" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E36" t="n">
-        <v>33.75625610351562</v>
+        <v>152.601957321167</v>
       </c>
       <c r="F36" t="n">
         <v>1</v>
@@ -1355,7 +1355,7 @@
     <row r="37">
       <c r="A37" s="1" t="inlineStr">
         <is>
-          <t>jqrs</t>
+          <t>gqrs</t>
         </is>
       </c>
       <c r="B37" s="1" t="n">
@@ -1386,19 +1386,19 @@
         <v>0.05</v>
       </c>
       <c r="C38" t="n">
-        <v>0.1765151515151516</v>
+        <v>0.4722442244224423</v>
       </c>
       <c r="D38" t="n">
         <v>0</v>
       </c>
       <c r="E38" t="n">
-        <v>1.493000000470784</v>
+        <v>60.72067022323608</v>
       </c>
       <c r="F38" t="n">
-        <v>0.1</v>
+        <v>0.7145909090909092</v>
       </c>
       <c r="G38" t="n">
-        <v>0.3280303030303031</v>
+        <v>0.3182739726027398</v>
       </c>
       <c r="H38" t="n">
         <v>29.99700029997</v>
@@ -1410,19 +1410,19 @@
         <v>0.25</v>
       </c>
       <c r="C39" t="n">
-        <v>0.7399797057331303</v>
+        <v>0.6666666666666666</v>
       </c>
       <c r="D39" t="n">
         <v>0</v>
       </c>
       <c r="E39" t="n">
-        <v>2.589000001549721</v>
+        <v>84.59854125976562</v>
       </c>
       <c r="F39" t="n">
-        <v>0.647456279809221</v>
+        <v>0.972972972972973</v>
       </c>
       <c r="G39" t="n">
-        <v>0.9565217391304348</v>
+        <v>0.5068493150684932</v>
       </c>
       <c r="H39" t="n">
         <v>60</v>
@@ -1434,19 +1434,19 @@
         <v>0.5</v>
       </c>
       <c r="C40" t="n">
-        <v>0.9459459459459459</v>
+        <v>0.8489256639530228</v>
       </c>
       <c r="D40" t="n">
         <v>0</v>
       </c>
       <c r="E40" t="n">
-        <v>3.050999999046326</v>
+        <v>120.7020282745361</v>
       </c>
       <c r="F40" t="n">
-        <v>0.9375</v>
+        <v>1</v>
       </c>
       <c r="G40" t="n">
-        <v>0.9743589743589743</v>
+        <v>0.8636363636363636</v>
       </c>
       <c r="H40" t="n">
         <v>72.0096012801707</v>
@@ -1458,13 +1458,13 @@
         <v>0.75</v>
       </c>
       <c r="C41" t="n">
-        <v>0.9875761837787154</v>
+        <v>0.9906542056074766</v>
       </c>
       <c r="D41" t="n">
         <v>0</v>
       </c>
       <c r="E41" t="n">
-        <v>3.282750001177192</v>
+        <v>134.2943906784058</v>
       </c>
       <c r="F41" t="n">
         <v>1</v>
@@ -1488,7 +1488,7 @@
         <v>0</v>
       </c>
       <c r="E42" t="n">
-        <v>3.930449997819959</v>
+        <v>142.3428535461426</v>
       </c>
       <c r="F42" t="n">
         <v>1</v>
@@ -1512,7 +1512,7 @@
         <v>1</v>
       </c>
       <c r="E43" t="n">
-        <v>48.47800000011921</v>
+        <v>158.9829921722412</v>
       </c>
       <c r="F43" t="n">
         <v>1</v>
@@ -1527,7 +1527,7 @@
     <row r="44">
       <c r="A44" s="1" t="inlineStr">
         <is>
-          <t>kali</t>
+          <t>hamilt</t>
         </is>
       </c>
       <c r="B44" s="1" t="n">
@@ -1540,7 +1540,7 @@
         <v>0</v>
       </c>
       <c r="E44" t="n">
-        <v>1.666069030761719</v>
+        <v>5.333900451660156</v>
       </c>
       <c r="F44" t="n">
         <v>0</v>
@@ -1564,7 +1564,7 @@
         <v>0</v>
       </c>
       <c r="E45" t="n">
-        <v>1.889228820800781</v>
+        <v>8.173215389251709</v>
       </c>
       <c r="F45" t="n">
         <v>0</v>
@@ -1582,19 +1582,19 @@
         <v>0.25</v>
       </c>
       <c r="C46" t="n">
-        <v>0.6666666666666666</v>
+        <v>0.7444140446876425</v>
       </c>
       <c r="D46" t="n">
         <v>0</v>
       </c>
       <c r="E46" t="n">
-        <v>2.079963684082031</v>
+        <v>10.96659898757935</v>
       </c>
       <c r="F46" t="n">
-        <v>0.8636363636363636</v>
+        <v>0.976328903654485</v>
       </c>
       <c r="G46" t="n">
-        <v>0.5471698113207547</v>
+        <v>0.6205555555555555</v>
       </c>
       <c r="H46" t="n">
         <v>60</v>
@@ -1606,19 +1606,19 @@
         <v>0.5</v>
       </c>
       <c r="C47" t="n">
-        <v>0.8888888888888888</v>
+        <v>0.9536672629695886</v>
       </c>
       <c r="D47" t="n">
         <v>0</v>
       </c>
       <c r="E47" t="n">
-        <v>2.283573150634766</v>
+        <v>16.76952838897705</v>
       </c>
       <c r="F47" t="n">
-        <v>0.9767441860465116</v>
+        <v>1</v>
       </c>
       <c r="G47" t="n">
-        <v>0.8333333333333334</v>
+        <v>0.9230769230769231</v>
       </c>
       <c r="H47" t="n">
         <v>72.0096012801707</v>
@@ -1630,19 +1630,19 @@
         <v>0.75</v>
       </c>
       <c r="C48" t="n">
-        <v>0.9859154929577465</v>
+        <v>0.9855072463768116</v>
       </c>
       <c r="D48" t="n">
         <v>0</v>
       </c>
       <c r="E48" t="n">
-        <v>2.429723739624023</v>
+        <v>19.13106441497803</v>
       </c>
       <c r="F48" t="n">
         <v>1</v>
       </c>
       <c r="G48" t="n">
-        <v>1</v>
+        <v>0.9741902834008097</v>
       </c>
       <c r="H48" t="n">
         <v>85.88309518125703</v>
@@ -1660,7 +1660,7 @@
         <v>0</v>
       </c>
       <c r="E49" t="n">
-        <v>4.243230819702148</v>
+        <v>21.23038768768311</v>
       </c>
       <c r="F49" t="n">
         <v>1</v>
@@ -1684,7 +1684,7 @@
         <v>0</v>
       </c>
       <c r="E50" t="n">
-        <v>31.32009506225586</v>
+        <v>27.92692184448242</v>
       </c>
       <c r="F50" t="n">
         <v>1</v>
@@ -1699,7 +1699,7 @@
     <row r="51">
       <c r="A51" s="1" t="inlineStr">
         <is>
-          <t>mart</t>
+          <t>jqrs</t>
         </is>
       </c>
       <c r="B51" s="1" t="n">
@@ -1712,7 +1712,7 @@
         <v>0</v>
       </c>
       <c r="E51" t="n">
-        <v>1.754045486450195</v>
+        <v>0</v>
       </c>
       <c r="F51" t="n">
         <v>0</v>
@@ -1730,19 +1730,19 @@
         <v>0.05</v>
       </c>
       <c r="C52" t="n">
-        <v>0</v>
+        <v>0.1765151515151516</v>
       </c>
       <c r="D52" t="n">
         <v>0</v>
       </c>
       <c r="E52" t="n">
-        <v>2.371847629547119</v>
+        <v>1.476649997383356</v>
       </c>
       <c r="F52" t="n">
-        <v>0</v>
+        <v>0.1</v>
       </c>
       <c r="G52" t="n">
-        <v>0</v>
+        <v>0.3280303030303031</v>
       </c>
       <c r="H52" t="n">
         <v>29.99700029997</v>
@@ -1754,19 +1754,19 @@
         <v>0.25</v>
       </c>
       <c r="C53" t="n">
-        <v>0</v>
+        <v>0.7399797057331303</v>
       </c>
       <c r="D53" t="n">
         <v>0</v>
       </c>
       <c r="E53" t="n">
-        <v>2.705156803131104</v>
+        <v>2.523749999701977</v>
       </c>
       <c r="F53" t="n">
-        <v>0</v>
+        <v>0.647456279809221</v>
       </c>
       <c r="G53" t="n">
-        <v>0</v>
+        <v>0.9565217391304348</v>
       </c>
       <c r="H53" t="n">
         <v>60</v>
@@ -1778,19 +1778,19 @@
         <v>0.5</v>
       </c>
       <c r="C54" t="n">
-        <v>0.2817460317460317</v>
+        <v>0.9459459459459459</v>
       </c>
       <c r="D54" t="n">
         <v>0</v>
       </c>
       <c r="E54" t="n">
-        <v>3.317594528198242</v>
+        <v>2.911499999463558</v>
       </c>
       <c r="F54" t="n">
-        <v>0.1762749445676275</v>
+        <v>0.9375</v>
       </c>
       <c r="G54" t="n">
-        <v>0.936491935483871</v>
+        <v>0.9743589743589743</v>
       </c>
       <c r="H54" t="n">
         <v>72.0096012801707</v>
@@ -1802,16 +1802,16 @@
         <v>0.75</v>
       </c>
       <c r="C55" t="n">
-        <v>0.9775193798449612</v>
+        <v>0.9875761837787154</v>
       </c>
       <c r="D55" t="n">
         <v>0</v>
       </c>
       <c r="E55" t="n">
-        <v>3.917217254638672</v>
+        <v>3.124749999493361</v>
       </c>
       <c r="F55" t="n">
-        <v>0.9776515151515152</v>
+        <v>1</v>
       </c>
       <c r="G55" t="n">
         <v>1</v>
@@ -1832,7 +1832,7 @@
         <v>0</v>
       </c>
       <c r="E56" t="n">
-        <v>5.250608921051024</v>
+        <v>3.637249999493359</v>
       </c>
       <c r="F56" t="n">
         <v>1</v>
@@ -1853,10 +1853,10 @@
         <v>1</v>
       </c>
       <c r="D57" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E57" t="n">
-        <v>24.80626106262207</v>
+        <v>53.7339999973774</v>
       </c>
       <c r="F57" t="n">
         <v>1</v>
@@ -1871,7 +1871,7 @@
     <row r="58">
       <c r="A58" s="1" t="inlineStr">
         <is>
-          <t>nab</t>
+          <t>kali</t>
         </is>
       </c>
       <c r="B58" s="1" t="n">
@@ -1884,7 +1884,7 @@
         <v>0</v>
       </c>
       <c r="E58" t="n">
-        <v>6.781816482543945</v>
+        <v>1.675128936767578</v>
       </c>
       <c r="F58" t="n">
         <v>0</v>
@@ -1902,19 +1902,19 @@
         <v>0.05</v>
       </c>
       <c r="C59" t="n">
-        <v>0.4444444444444444</v>
+        <v>0</v>
       </c>
       <c r="D59" t="n">
         <v>0</v>
       </c>
       <c r="E59" t="n">
-        <v>12.54597902297974</v>
+        <v>1.883184909820557</v>
       </c>
       <c r="F59" t="n">
-        <v>0.3564849624060151</v>
+        <v>0</v>
       </c>
       <c r="G59" t="n">
-        <v>0.6046428571428571</v>
+        <v>0</v>
       </c>
       <c r="H59" t="n">
         <v>29.99700029997</v>
@@ -1926,19 +1926,19 @@
         <v>0.25</v>
       </c>
       <c r="C60" t="n">
-        <v>0.8065930956423316</v>
+        <v>0.6666666666666666</v>
       </c>
       <c r="D60" t="n">
         <v>0</v>
       </c>
       <c r="E60" t="n">
-        <v>18.54419708251953</v>
+        <v>1.99204683303833</v>
       </c>
       <c r="F60" t="n">
-        <v>0.7272727272727273</v>
+        <v>0.8636363636363636</v>
       </c>
       <c r="G60" t="n">
-        <v>0.95</v>
+        <v>0.5471698113207547</v>
       </c>
       <c r="H60" t="n">
         <v>60</v>
@@ -1950,19 +1950,19 @@
         <v>0.5</v>
       </c>
       <c r="C61" t="n">
-        <v>0.9459459459459459</v>
+        <v>0.8888888888888888</v>
       </c>
       <c r="D61" t="n">
         <v>0</v>
       </c>
       <c r="E61" t="n">
-        <v>25.49302577972412</v>
+        <v>2.162933349609375</v>
       </c>
       <c r="F61" t="n">
-        <v>0.925</v>
+        <v>0.9767441860465116</v>
       </c>
       <c r="G61" t="n">
-        <v>1</v>
+        <v>0.8333333333333334</v>
       </c>
       <c r="H61" t="n">
         <v>72.0096012801707</v>
@@ -1974,16 +1974,16 @@
         <v>0.75</v>
       </c>
       <c r="C62" t="n">
-        <v>0.9836065573770492</v>
+        <v>0.9859154929577465</v>
       </c>
       <c r="D62" t="n">
         <v>0</v>
       </c>
       <c r="E62" t="n">
-        <v>25.86674690246582</v>
+        <v>2.250909805297852</v>
       </c>
       <c r="F62" t="n">
-        <v>0.9714285714285714</v>
+        <v>1</v>
       </c>
       <c r="G62" t="n">
         <v>1</v>
@@ -1998,13 +1998,13 @@
         <v>0.95</v>
       </c>
       <c r="C63" t="n">
-        <v>0.9895496473141616</v>
+        <v>1</v>
       </c>
       <c r="D63" t="n">
         <v>0</v>
       </c>
       <c r="E63" t="n">
-        <v>26.46478414535522</v>
+        <v>2.416729927062988</v>
       </c>
       <c r="F63" t="n">
         <v>1</v>
@@ -2028,7 +2028,7 @@
         <v>0</v>
       </c>
       <c r="E64" t="n">
-        <v>33.80465507507324</v>
+        <v>14.11795616149902</v>
       </c>
       <c r="F64" t="n">
         <v>1</v>
@@ -2043,7 +2043,7 @@
     <row r="65">
       <c r="A65" s="1" t="inlineStr">
         <is>
-          <t>nk</t>
+          <t>mart</t>
         </is>
       </c>
       <c r="B65" s="1" t="n">
@@ -2056,7 +2056,7 @@
         <v>0</v>
       </c>
       <c r="E65" t="n">
-        <v>2.09498405456543</v>
+        <v>1.711130142211914</v>
       </c>
       <c r="F65" t="n">
         <v>0</v>
@@ -2074,19 +2074,19 @@
         <v>0.05</v>
       </c>
       <c r="C66" t="n">
-        <v>0.7192820512820512</v>
+        <v>0</v>
       </c>
       <c r="D66" t="n">
         <v>0</v>
       </c>
       <c r="E66" t="n">
-        <v>2.288103103637695</v>
+        <v>2.336025238037109</v>
       </c>
       <c r="F66" t="n">
-        <v>0.7676470588235295</v>
+        <v>0</v>
       </c>
       <c r="G66" t="n">
-        <v>0.6930000000000001</v>
+        <v>0</v>
       </c>
       <c r="H66" t="n">
         <v>29.99700029997</v>
@@ -2098,19 +2098,19 @@
         <v>0.25</v>
       </c>
       <c r="C67" t="n">
-        <v>0.9591780821917808</v>
+        <v>0</v>
       </c>
       <c r="D67" t="n">
         <v>0</v>
       </c>
       <c r="E67" t="n">
-        <v>2.531230449676514</v>
+        <v>2.689719200134277</v>
       </c>
       <c r="F67" t="n">
-        <v>0.9710144927536232</v>
+        <v>0</v>
       </c>
       <c r="G67" t="n">
-        <v>0.9591836734693877</v>
+        <v>0</v>
       </c>
       <c r="H67" t="n">
         <v>60</v>
@@ -2122,19 +2122,19 @@
         <v>0.5</v>
       </c>
       <c r="C68" t="n">
-        <v>0.9866666666666667</v>
+        <v>0.2817460317460317</v>
       </c>
       <c r="D68" t="n">
         <v>0</v>
       </c>
       <c r="E68" t="n">
-        <v>2.721071243286133</v>
+        <v>3.258943557739258</v>
       </c>
       <c r="F68" t="n">
-        <v>1</v>
+        <v>0.1762749445676275</v>
       </c>
       <c r="G68" t="n">
-        <v>1</v>
+        <v>0.936491935483871</v>
       </c>
       <c r="H68" t="n">
         <v>72.0096012801707</v>
@@ -2146,16 +2146,16 @@
         <v>0.75</v>
       </c>
       <c r="C69" t="n">
-        <v>1</v>
+        <v>0.9775193798449612</v>
       </c>
       <c r="D69" t="n">
         <v>0</v>
       </c>
       <c r="E69" t="n">
-        <v>2.892732620239258</v>
+        <v>3.730952739715576</v>
       </c>
       <c r="F69" t="n">
-        <v>1</v>
+        <v>0.9776515151515152</v>
       </c>
       <c r="G69" t="n">
         <v>1</v>
@@ -2176,7 +2176,7 @@
         <v>0</v>
       </c>
       <c r="E70" t="n">
-        <v>3.29867601394653</v>
+        <v>4.696130752563477</v>
       </c>
       <c r="F70" t="n">
         <v>1</v>
@@ -2200,7 +2200,7 @@
         <v>0</v>
       </c>
       <c r="E71" t="n">
-        <v>7.384061813354492</v>
+        <v>22.63689041137695</v>
       </c>
       <c r="F71" t="n">
         <v>1</v>
@@ -2215,7 +2215,7 @@
     <row r="72">
       <c r="A72" s="1" t="inlineStr">
         <is>
-          <t>pan-tomp</t>
+          <t>nab</t>
         </is>
       </c>
       <c r="B72" s="1" t="n">
@@ -2228,7 +2228,7 @@
         <v>0</v>
       </c>
       <c r="E72" t="n">
-        <v>1.234292984008789</v>
+        <v>7.056951522827148</v>
       </c>
       <c r="F72" t="n">
         <v>0</v>
@@ -2246,19 +2246,19 @@
         <v>0.05</v>
       </c>
       <c r="C73" t="n">
-        <v>0</v>
+        <v>0.4444444444444444</v>
       </c>
       <c r="D73" t="n">
         <v>0</v>
       </c>
       <c r="E73" t="n">
-        <v>1.362955570220947</v>
+        <v>12.92506456375122</v>
       </c>
       <c r="F73" t="n">
-        <v>0</v>
+        <v>0.3564849624060151</v>
       </c>
       <c r="G73" t="n">
-        <v>0</v>
+        <v>0.6046428571428571</v>
       </c>
       <c r="H73" t="n">
         <v>29.99700029997</v>
@@ -2270,19 +2270,19 @@
         <v>0.25</v>
       </c>
       <c r="C74" t="n">
-        <v>0.6715292903817494</v>
+        <v>0.8065930956423316</v>
       </c>
       <c r="D74" t="n">
         <v>0</v>
       </c>
       <c r="E74" t="n">
-        <v>1.804351806640625</v>
+        <v>18.4590220451355</v>
       </c>
       <c r="F74" t="n">
-        <v>0.9781249999999999</v>
+        <v>0.7272727272727273</v>
       </c>
       <c r="G74" t="n">
-        <v>0.5258859784283514</v>
+        <v>0.95</v>
       </c>
       <c r="H74" t="n">
         <v>60</v>
@@ -2294,19 +2294,19 @@
         <v>0.5</v>
       </c>
       <c r="C75" t="n">
-        <v>0.9508196721311475</v>
+        <v>0.9459459459459459</v>
       </c>
       <c r="D75" t="n">
         <v>0</v>
       </c>
       <c r="E75" t="n">
-        <v>2.243518829345703</v>
+        <v>25.61104297637939</v>
       </c>
       <c r="F75" t="n">
-        <v>1</v>
+        <v>0.925</v>
       </c>
       <c r="G75" t="n">
-        <v>0.911437908496732</v>
+        <v>1</v>
       </c>
       <c r="H75" t="n">
         <v>72.0096012801707</v>
@@ -2318,19 +2318,19 @@
         <v>0.75</v>
       </c>
       <c r="C76" t="n">
-        <v>0.9859154929577465</v>
+        <v>0.9836065573770492</v>
       </c>
       <c r="D76" t="n">
         <v>0</v>
       </c>
       <c r="E76" t="n">
-        <v>2.484798431396484</v>
+        <v>26.13800764083862</v>
       </c>
       <c r="F76" t="n">
-        <v>1</v>
+        <v>0.9714285714285714</v>
       </c>
       <c r="G76" t="n">
-        <v>0.9849598163030999</v>
+        <v>1</v>
       </c>
       <c r="H76" t="n">
         <v>85.88309518125703</v>
@@ -2342,13 +2342,13 @@
         <v>0.95</v>
       </c>
       <c r="C77" t="n">
-        <v>1</v>
+        <v>0.9895496473141616</v>
       </c>
       <c r="D77" t="n">
         <v>0</v>
       </c>
       <c r="E77" t="n">
-        <v>2.801764011383057</v>
+        <v>26.99217796325684</v>
       </c>
       <c r="F77" t="n">
         <v>1</v>
@@ -2372,7 +2372,7 @@
         <v>0</v>
       </c>
       <c r="E78" t="n">
-        <v>4.097223281860352</v>
+        <v>36.86189651489258</v>
       </c>
       <c r="F78" t="n">
         <v>1</v>
@@ -2387,7 +2387,7 @@
     <row r="79">
       <c r="A79" s="1" t="inlineStr">
         <is>
-          <t>rdeco</t>
+          <t>nk</t>
         </is>
       </c>
       <c r="B79" s="1" t="n">
@@ -2400,7 +2400,7 @@
         <v>0</v>
       </c>
       <c r="E79" t="n">
-        <v>0</v>
+        <v>2.114057540893555</v>
       </c>
       <c r="F79" t="n">
         <v>0</v>
@@ -2418,19 +2418,19 @@
         <v>0.05</v>
       </c>
       <c r="C80" t="n">
-        <v>0.2339285714285717</v>
+        <v>0.7192820512820512</v>
       </c>
       <c r="D80" t="n">
         <v>0</v>
       </c>
       <c r="E80" t="n">
-        <v>1.7992999994196</v>
+        <v>2.289128303527832</v>
       </c>
       <c r="F80" t="n">
-        <v>0.5</v>
+        <v>0.7676470588235295</v>
       </c>
       <c r="G80" t="n">
-        <v>0.1536111111111111</v>
+        <v>0.6930000000000001</v>
       </c>
       <c r="H80" t="n">
         <v>29.99700029997</v>
@@ -2442,19 +2442,19 @@
         <v>0.25</v>
       </c>
       <c r="C81" t="n">
-        <v>0.925</v>
+        <v>0.9591780821917808</v>
       </c>
       <c r="D81" t="n">
         <v>0</v>
       </c>
       <c r="E81" t="n">
-        <v>2.188000001013279</v>
+        <v>2.493202686309814</v>
       </c>
       <c r="F81" t="n">
-        <v>0.9565217391304348</v>
+        <v>0.9710144927536232</v>
       </c>
       <c r="G81" t="n">
-        <v>0.9115942028985506</v>
+        <v>0.9591836734693877</v>
       </c>
       <c r="H81" t="n">
         <v>60</v>
@@ -2466,19 +2466,19 @@
         <v>0.5</v>
       </c>
       <c r="C82" t="n">
-        <v>0.9803921568627451</v>
+        <v>0.9866666666666667</v>
       </c>
       <c r="D82" t="n">
         <v>0</v>
       </c>
       <c r="E82" t="n">
-        <v>2.438499998301268</v>
+        <v>2.645015716552734</v>
       </c>
       <c r="F82" t="n">
         <v>1</v>
       </c>
       <c r="G82" t="n">
-        <v>0.975</v>
+        <v>1</v>
       </c>
       <c r="H82" t="n">
         <v>72.0096012801707</v>
@@ -2496,7 +2496,7 @@
         <v>0</v>
       </c>
       <c r="E83" t="n">
-        <v>2.983499999158084</v>
+        <v>2.791881561279297</v>
       </c>
       <c r="F83" t="n">
         <v>1</v>
@@ -2520,7 +2520,7 @@
         <v>0</v>
       </c>
       <c r="E84" t="n">
-        <v>6.400450000446289</v>
+        <v>3.128969669342041</v>
       </c>
       <c r="F84" t="n">
         <v>1</v>
@@ -2541,10 +2541,10 @@
         <v>1</v>
       </c>
       <c r="D85" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E85" t="n">
-        <v>27.7690000012517</v>
+        <v>3.875970840454102</v>
       </c>
       <c r="F85" t="n">
         <v>1</v>
@@ -2559,7 +2559,7 @@
     <row r="86">
       <c r="A86" s="1" t="inlineStr">
         <is>
-          <t>rpeak</t>
+          <t>pan-tomp</t>
         </is>
       </c>
       <c r="B86" s="1" t="n">
@@ -2572,7 +2572,7 @@
         <v>0</v>
       </c>
       <c r="E86" t="n">
-        <v>0</v>
+        <v>1.2359619140625</v>
       </c>
       <c r="F86" t="n">
         <v>0</v>
@@ -2596,7 +2596,7 @@
         <v>0</v>
       </c>
       <c r="E87" t="n">
-        <v>0.6260000001231674</v>
+        <v>1.332998275756836</v>
       </c>
       <c r="F87" t="n">
         <v>0</v>
@@ -2614,19 +2614,19 @@
         <v>0.25</v>
       </c>
       <c r="C88" t="n">
-        <v>0.2673208682845617</v>
+        <v>0.6715292903817494</v>
       </c>
       <c r="D88" t="n">
         <v>0</v>
       </c>
       <c r="E88" t="n">
-        <v>0.8672500043176115</v>
+        <v>1.651287078857422</v>
       </c>
       <c r="F88" t="n">
-        <v>0.945933014354067</v>
+        <v>0.9781249999999999</v>
       </c>
       <c r="G88" t="n">
-        <v>0.1716376898481215</v>
+        <v>0.5258859784283514</v>
       </c>
       <c r="H88" t="n">
         <v>60</v>
@@ -2638,19 +2638,19 @@
         <v>0.5</v>
       </c>
       <c r="C89" t="n">
-        <v>0.6063089915548932</v>
+        <v>0.9508196721311475</v>
       </c>
       <c r="D89" t="n">
         <v>0</v>
       </c>
       <c r="E89" t="n">
-        <v>1.040000000037253</v>
+        <v>2.035021781921387</v>
       </c>
       <c r="F89" t="n">
         <v>1</v>
       </c>
       <c r="G89" t="n">
-        <v>0.521286231884058</v>
+        <v>0.911437908496732</v>
       </c>
       <c r="H89" t="n">
         <v>72.0096012801707</v>
@@ -2662,19 +2662,19 @@
         <v>0.75</v>
       </c>
       <c r="C90" t="n">
-        <v>0.9844932844932845</v>
+        <v>0.9859154929577465</v>
       </c>
       <c r="D90" t="n">
         <v>0</v>
       </c>
       <c r="E90" t="n">
-        <v>1.471000000834465</v>
+        <v>2.283036708831787</v>
       </c>
       <c r="F90" t="n">
         <v>1</v>
       </c>
       <c r="G90" t="n">
-        <v>0.9772727272727273</v>
+        <v>0.9849598163030999</v>
       </c>
       <c r="H90" t="n">
         <v>85.88309518125703</v>
@@ -2692,7 +2692,7 @@
         <v>0</v>
       </c>
       <c r="E91" t="n">
-        <v>1.97135000154376</v>
+        <v>2.688336372375487</v>
       </c>
       <c r="F91" t="n">
         <v>1</v>
@@ -2713,10 +2713,10 @@
         <v>1</v>
       </c>
       <c r="D92" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E92" t="n">
-        <v>17.2390000000596</v>
+        <v>5.067110061645508</v>
       </c>
       <c r="F92" t="n">
         <v>1</v>
@@ -2731,7 +2731,7 @@
     <row r="93">
       <c r="A93" s="1" t="inlineStr">
         <is>
-          <t>two-avg</t>
+          <t>rdeco</t>
         </is>
       </c>
       <c r="B93" s="1" t="n">
@@ -2744,7 +2744,7 @@
         <v>0</v>
       </c>
       <c r="E93" t="n">
-        <v>2.932071685791016</v>
+        <v>0</v>
       </c>
       <c r="F93" t="n">
         <v>0</v>
@@ -2762,19 +2762,19 @@
         <v>0.05</v>
       </c>
       <c r="C94" t="n">
-        <v>0.7172395557905871</v>
+        <v>0.2339285714285717</v>
       </c>
       <c r="D94" t="n">
         <v>0</v>
       </c>
       <c r="E94" t="n">
-        <v>5.411064624786377</v>
+        <v>1.753849998116493</v>
       </c>
       <c r="F94" t="n">
-        <v>0.9230769230769231</v>
+        <v>0.5</v>
       </c>
       <c r="G94" t="n">
-        <v>0.5618357487922706</v>
+        <v>0.1536111111111111</v>
       </c>
       <c r="H94" t="n">
         <v>29.99700029997</v>
@@ -2786,19 +2786,19 @@
         <v>0.25</v>
       </c>
       <c r="C95" t="n">
-        <v>0.9428571428571428</v>
+        <v>0.925</v>
       </c>
       <c r="D95" t="n">
         <v>0</v>
       </c>
       <c r="E95" t="n">
-        <v>6.798803806304932</v>
+        <v>2.103999990038574</v>
       </c>
       <c r="F95" t="n">
-        <v>0.9757549361207898</v>
+        <v>0.9565217391304348</v>
       </c>
       <c r="G95" t="n">
-        <v>0.9090909090909091</v>
+        <v>0.9115942028985506</v>
       </c>
       <c r="H95" t="n">
         <v>60</v>
@@ -2810,19 +2810,19 @@
         <v>0.5</v>
       </c>
       <c r="C96" t="n">
-        <v>0.9855072463768116</v>
+        <v>0.9803921568627451</v>
       </c>
       <c r="D96" t="n">
         <v>0</v>
       </c>
       <c r="E96" t="n">
-        <v>9.033441543579102</v>
+        <v>2.310000002384186</v>
       </c>
       <c r="F96" t="n">
         <v>1</v>
       </c>
       <c r="G96" t="n">
-        <v>1</v>
+        <v>0.975</v>
       </c>
       <c r="H96" t="n">
         <v>72.0096012801707</v>
@@ -2840,7 +2840,7 @@
         <v>0</v>
       </c>
       <c r="E97" t="n">
-        <v>9.128272533416748</v>
+        <v>2.718499997630715</v>
       </c>
       <c r="F97" t="n">
         <v>1</v>
@@ -2864,7 +2864,7 @@
         <v>0</v>
       </c>
       <c r="E98" t="n">
-        <v>9.864449501037598</v>
+        <v>4.760399999842047</v>
       </c>
       <c r="F98" t="n">
         <v>1</v>
@@ -2885,10 +2885,10 @@
         <v>1</v>
       </c>
       <c r="D99" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E99" t="n">
-        <v>11.87396049499512</v>
+        <v>30.26700000092387</v>
       </c>
       <c r="F99" t="n">
         <v>1</v>
@@ -2903,7 +2903,7 @@
     <row r="100">
       <c r="A100" s="1" t="inlineStr">
         <is>
-          <t>unsw</t>
+          <t>rpeak</t>
         </is>
       </c>
       <c r="B100" s="1" t="n">
@@ -2916,7 +2916,7 @@
         <v>0</v>
       </c>
       <c r="E100" t="n">
-        <v>8.366999998688698</v>
+        <v>0</v>
       </c>
       <c r="F100" t="n">
         <v>0</v>
@@ -2934,19 +2934,19 @@
         <v>0.05</v>
       </c>
       <c r="C101" t="n">
-        <v>0.6958314034275129</v>
+        <v>0</v>
       </c>
       <c r="D101" t="n">
         <v>0</v>
       </c>
       <c r="E101" t="n">
-        <v>12.15984999995562</v>
+        <v>0.6206500012427568</v>
       </c>
       <c r="F101" t="n">
-        <v>0.8991025641025642</v>
+        <v>0</v>
       </c>
       <c r="G101" t="n">
-        <v>0.5731907894736843</v>
+        <v>0</v>
       </c>
       <c r="H101" t="n">
         <v>29.99700029997</v>
@@ -2958,19 +2958,19 @@
         <v>0.25</v>
       </c>
       <c r="C102" t="n">
-        <v>0.9696969696969697</v>
+        <v>0.2673208682845617</v>
       </c>
       <c r="D102" t="n">
         <v>0</v>
       </c>
       <c r="E102" t="n">
-        <v>18.17775000073016</v>
+        <v>0.8149999981978908</v>
       </c>
       <c r="F102" t="n">
-        <v>1</v>
+        <v>0.945933014354067</v>
       </c>
       <c r="G102" t="n">
-        <v>0.9523809523809523</v>
+        <v>0.1716376898481215</v>
       </c>
       <c r="H102" t="n">
         <v>60</v>
@@ -2982,19 +2982,19 @@
         <v>0.5</v>
       </c>
       <c r="C103" t="n">
-        <v>0.9873417721518988</v>
+        <v>0.6063089915548932</v>
       </c>
       <c r="D103" t="n">
         <v>0</v>
       </c>
       <c r="E103" t="n">
-        <v>36.82699999865144</v>
+        <v>0.9660000037401915</v>
       </c>
       <c r="F103" t="n">
         <v>1</v>
       </c>
       <c r="G103" t="n">
-        <v>0.9782608695652174</v>
+        <v>0.521286231884058</v>
       </c>
       <c r="H103" t="n">
         <v>72.0096012801707</v>
@@ -3006,19 +3006,19 @@
         <v>0.75</v>
       </c>
       <c r="C104" t="n">
-        <v>1</v>
+        <v>0.9844932844932845</v>
       </c>
       <c r="D104" t="n">
         <v>0</v>
       </c>
       <c r="E104" t="n">
-        <v>39.12900000018999</v>
+        <v>1.35050000436604</v>
       </c>
       <c r="F104" t="n">
         <v>1</v>
       </c>
       <c r="G104" t="n">
-        <v>1</v>
+        <v>0.9772727272727273</v>
       </c>
       <c r="H104" t="n">
         <v>85.88309518125703</v>
@@ -3036,7 +3036,7 @@
         <v>0</v>
       </c>
       <c r="E105" t="n">
-        <v>45.38795000091195</v>
+        <v>1.841750001907348</v>
       </c>
       <c r="F105" t="n">
         <v>1</v>
@@ -3057,10 +3057,10 @@
         <v>1</v>
       </c>
       <c r="D106" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E106" t="n">
-        <v>75.85600000061095</v>
+        <v>8.802999999374151</v>
       </c>
       <c r="F106" t="n">
         <v>1</v>
@@ -3075,7 +3075,7 @@
     <row r="107">
       <c r="A107" s="1" t="inlineStr">
         <is>
-          <t>wqrs</t>
+          <t>two-avg</t>
         </is>
       </c>
       <c r="B107" s="1" t="n">
@@ -3088,7 +3088,7 @@
         <v>0</v>
       </c>
       <c r="E107" t="n">
-        <v>63.14706802368164</v>
+        <v>2.819061279296875</v>
       </c>
       <c r="F107" t="n">
         <v>0</v>
@@ -3106,19 +3106,19 @@
         <v>0.05</v>
       </c>
       <c r="C108" t="n">
-        <v>0.4259398496240602</v>
+        <v>0.7172395557905871</v>
       </c>
       <c r="D108" t="n">
         <v>0</v>
       </c>
       <c r="E108" t="n">
-        <v>126.787805557251</v>
+        <v>5.181944370269775</v>
       </c>
       <c r="F108" t="n">
-        <v>0.6</v>
+        <v>0.9230769230769231</v>
       </c>
       <c r="G108" t="n">
-        <v>0.3846153846153846</v>
+        <v>0.5618357487922706</v>
       </c>
       <c r="H108" t="n">
         <v>29.99700029997</v>
@@ -3130,19 +3130,19 @@
         <v>0.25</v>
       </c>
       <c r="C109" t="n">
-        <v>0.7567567567567568</v>
+        <v>0.9428571428571428</v>
       </c>
       <c r="D109" t="n">
         <v>0</v>
       </c>
       <c r="E109" t="n">
-        <v>185.9567761421204</v>
+        <v>6.720185279846191</v>
       </c>
       <c r="F109" t="n">
-        <v>0.8521241830065359</v>
+        <v>0.9757549361207898</v>
       </c>
       <c r="G109" t="n">
-        <v>0.6818181818181818</v>
+        <v>0.9090909090909091</v>
       </c>
       <c r="H109" t="n">
         <v>60</v>
@@ -3154,19 +3154,19 @@
         <v>0.5</v>
       </c>
       <c r="C110" t="n">
-        <v>0.8979933110367893</v>
+        <v>0.9855072463768116</v>
       </c>
       <c r="D110" t="n">
         <v>0</v>
       </c>
       <c r="E110" t="n">
-        <v>258.938193321228</v>
+        <v>9.031414985656738</v>
       </c>
       <c r="F110" t="n">
         <v>1</v>
       </c>
       <c r="G110" t="n">
-        <v>0.9028324154209284</v>
+        <v>1</v>
       </c>
       <c r="H110" t="n">
         <v>72.0096012801707</v>
@@ -3178,19 +3178,19 @@
         <v>0.75</v>
       </c>
       <c r="C111" t="n">
-        <v>0.9761904761904762</v>
+        <v>1</v>
       </c>
       <c r="D111" t="n">
         <v>0</v>
       </c>
       <c r="E111" t="n">
-        <v>261.0234618186951</v>
+        <v>9.209811687469482</v>
       </c>
       <c r="F111" t="n">
         <v>1</v>
       </c>
       <c r="G111" t="n">
-        <v>0.9736842105263158</v>
+        <v>1</v>
       </c>
       <c r="H111" t="n">
         <v>85.88309518125703</v>
@@ -3202,13 +3202,13 @@
         <v>0.95</v>
       </c>
       <c r="C112" t="n">
-        <v>0.9923686477174849</v>
+        <v>1</v>
       </c>
       <c r="D112" t="n">
         <v>0</v>
       </c>
       <c r="E112" t="n">
-        <v>265.5675768852234</v>
+        <v>9.521198272705076</v>
       </c>
       <c r="F112" t="n">
         <v>1</v>
@@ -3232,7 +3232,7 @@
         <v>0</v>
       </c>
       <c r="E113" t="n">
-        <v>382.7800750732422</v>
+        <v>9.8419189453125</v>
       </c>
       <c r="F113" t="n">
         <v>1</v>
@@ -3244,8 +3244,352 @@
         <v>168</v>
       </c>
     </row>
+    <row r="114">
+      <c r="A114" s="1" t="inlineStr">
+        <is>
+          <t>unsw</t>
+        </is>
+      </c>
+      <c r="B114" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="C114" t="n">
+        <v>0</v>
+      </c>
+      <c r="D114" t="n">
+        <v>0</v>
+      </c>
+      <c r="E114" t="n">
+        <v>8.315999999642372</v>
+      </c>
+      <c r="F114" t="n">
+        <v>0</v>
+      </c>
+      <c r="G114" t="n">
+        <v>0</v>
+      </c>
+      <c r="H114" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="115">
+      <c r="A115" s="1" t="n"/>
+      <c r="B115" s="1" t="n">
+        <v>0.05</v>
+      </c>
+      <c r="C115" t="n">
+        <v>0.6958314034275129</v>
+      </c>
+      <c r="D115" t="n">
+        <v>0</v>
+      </c>
+      <c r="E115" t="n">
+        <v>12.2229499951005</v>
+      </c>
+      <c r="F115" t="n">
+        <v>0.8991025641025642</v>
+      </c>
+      <c r="G115" t="n">
+        <v>0.5731907894736843</v>
+      </c>
+      <c r="H115" t="n">
+        <v>29.99700029997</v>
+      </c>
+    </row>
+    <row r="116">
+      <c r="A116" s="1" t="n"/>
+      <c r="B116" s="1" t="n">
+        <v>0.25</v>
+      </c>
+      <c r="C116" t="n">
+        <v>0.9696969696969697</v>
+      </c>
+      <c r="D116" t="n">
+        <v>0</v>
+      </c>
+      <c r="E116" t="n">
+        <v>18.21375000290573</v>
+      </c>
+      <c r="F116" t="n">
+        <v>1</v>
+      </c>
+      <c r="G116" t="n">
+        <v>0.9523809523809523</v>
+      </c>
+      <c r="H116" t="n">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="117">
+      <c r="A117" s="1" t="n"/>
+      <c r="B117" s="1" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="C117" t="n">
+        <v>0.9873417721518988</v>
+      </c>
+      <c r="D117" t="n">
+        <v>0</v>
+      </c>
+      <c r="E117" t="n">
+        <v>37.83449999988079</v>
+      </c>
+      <c r="F117" t="n">
+        <v>1</v>
+      </c>
+      <c r="G117" t="n">
+        <v>0.9782608695652174</v>
+      </c>
+      <c r="H117" t="n">
+        <v>72.0096012801707</v>
+      </c>
+    </row>
+    <row r="118">
+      <c r="A118" s="1" t="n"/>
+      <c r="B118" s="1" t="n">
+        <v>0.75</v>
+      </c>
+      <c r="C118" t="n">
+        <v>1</v>
+      </c>
+      <c r="D118" t="n">
+        <v>0</v>
+      </c>
+      <c r="E118" t="n">
+        <v>40.69000000320375</v>
+      </c>
+      <c r="F118" t="n">
+        <v>1</v>
+      </c>
+      <c r="G118" t="n">
+        <v>1</v>
+      </c>
+      <c r="H118" t="n">
+        <v>85.88309518125703</v>
+      </c>
+    </row>
+    <row r="119">
+      <c r="A119" s="1" t="n"/>
+      <c r="B119" s="1" t="n">
+        <v>0.95</v>
+      </c>
+      <c r="C119" t="n">
+        <v>1</v>
+      </c>
+      <c r="D119" t="n">
+        <v>0</v>
+      </c>
+      <c r="E119" t="n">
+        <v>48.10405000336468</v>
+      </c>
+      <c r="F119" t="n">
+        <v>1</v>
+      </c>
+      <c r="G119" t="n">
+        <v>1</v>
+      </c>
+      <c r="H119" t="n">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="120">
+      <c r="A120" s="1" t="n"/>
+      <c r="B120" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="C120" t="n">
+        <v>1</v>
+      </c>
+      <c r="D120" t="n">
+        <v>0</v>
+      </c>
+      <c r="E120" t="n">
+        <v>106.1840000003576</v>
+      </c>
+      <c r="F120" t="n">
+        <v>1</v>
+      </c>
+      <c r="G120" t="n">
+        <v>1</v>
+      </c>
+      <c r="H120" t="n">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="121">
+      <c r="A121" s="1" t="inlineStr">
+        <is>
+          <t>wqrs</t>
+        </is>
+      </c>
+      <c r="B121" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="C121" t="n">
+        <v>0</v>
+      </c>
+      <c r="D121" t="n">
+        <v>0</v>
+      </c>
+      <c r="E121" t="n">
+        <v>64.55612182617188</v>
+      </c>
+      <c r="F121" t="n">
+        <v>0</v>
+      </c>
+      <c r="G121" t="n">
+        <v>0</v>
+      </c>
+      <c r="H121" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="122">
+      <c r="A122" s="1" t="n"/>
+      <c r="B122" s="1" t="n">
+        <v>0.05</v>
+      </c>
+      <c r="C122" t="n">
+        <v>0.4259398496240602</v>
+      </c>
+      <c r="D122" t="n">
+        <v>0</v>
+      </c>
+      <c r="E122" t="n">
+        <v>129.6574711799622</v>
+      </c>
+      <c r="F122" t="n">
+        <v>0.6</v>
+      </c>
+      <c r="G122" t="n">
+        <v>0.3846153846153846</v>
+      </c>
+      <c r="H122" t="n">
+        <v>29.99700029997</v>
+      </c>
+    </row>
+    <row r="123">
+      <c r="A123" s="1" t="n"/>
+      <c r="B123" s="1" t="n">
+        <v>0.25</v>
+      </c>
+      <c r="C123" t="n">
+        <v>0.7567567567567568</v>
+      </c>
+      <c r="D123" t="n">
+        <v>0</v>
+      </c>
+      <c r="E123" t="n">
+        <v>184.79984998703</v>
+      </c>
+      <c r="F123" t="n">
+        <v>0.8521241830065359</v>
+      </c>
+      <c r="G123" t="n">
+        <v>0.6818181818181818</v>
+      </c>
+      <c r="H123" t="n">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="124">
+      <c r="A124" s="1" t="n"/>
+      <c r="B124" s="1" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="C124" t="n">
+        <v>0.8979933110367893</v>
+      </c>
+      <c r="D124" t="n">
+        <v>0</v>
+      </c>
+      <c r="E124" t="n">
+        <v>256.0614347457886</v>
+      </c>
+      <c r="F124" t="n">
+        <v>1</v>
+      </c>
+      <c r="G124" t="n">
+        <v>0.9028324154209284</v>
+      </c>
+      <c r="H124" t="n">
+        <v>72.0096012801707</v>
+      </c>
+    </row>
+    <row r="125">
+      <c r="A125" s="1" t="n"/>
+      <c r="B125" s="1" t="n">
+        <v>0.75</v>
+      </c>
+      <c r="C125" t="n">
+        <v>0.9761904761904762</v>
+      </c>
+      <c r="D125" t="n">
+        <v>0</v>
+      </c>
+      <c r="E125" t="n">
+        <v>259.9309682846069</v>
+      </c>
+      <c r="F125" t="n">
+        <v>1</v>
+      </c>
+      <c r="G125" t="n">
+        <v>0.9736842105263158</v>
+      </c>
+      <c r="H125" t="n">
+        <v>85.88309518125703</v>
+      </c>
+    </row>
+    <row r="126">
+      <c r="A126" s="1" t="n"/>
+      <c r="B126" s="1" t="n">
+        <v>0.95</v>
+      </c>
+      <c r="C126" t="n">
+        <v>0.9923686477174849</v>
+      </c>
+      <c r="D126" t="n">
+        <v>0</v>
+      </c>
+      <c r="E126" t="n">
+        <v>266.3999915122986</v>
+      </c>
+      <c r="F126" t="n">
+        <v>1</v>
+      </c>
+      <c r="G126" t="n">
+        <v>1</v>
+      </c>
+      <c r="H126" t="n">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="127">
+      <c r="A127" s="1" t="n"/>
+      <c r="B127" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="C127" t="n">
+        <v>1</v>
+      </c>
+      <c r="D127" t="n">
+        <v>0</v>
+      </c>
+      <c r="E127" t="n">
+        <v>955452.7499675751</v>
+      </c>
+      <c r="F127" t="n">
+        <v>1</v>
+      </c>
+      <c r="G127" t="n">
+        <v>1</v>
+      </c>
+      <c r="H127" t="n">
+        <v>168</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="16">
+  <mergeCells count="18">
     <mergeCell ref="A2:A8"/>
     <mergeCell ref="A9:A15"/>
     <mergeCell ref="A16:A22"/>
@@ -3262,6 +3606,8 @@
     <mergeCell ref="A93:A99"/>
     <mergeCell ref="A100:A106"/>
     <mergeCell ref="A107:A113"/>
+    <mergeCell ref="A114:A120"/>
+    <mergeCell ref="A121:A127"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
results from running assessment of 18 beat detectors
finished assessment on 09-Jan-2024. I think the version of main_pc.ipynb which was used had been committed previously.
</commit_message>
<xml_diff>
--- a/Algorithm_tester/data_autosave/real_overall.xlsx
+++ b/Algorithm_tester/data_autosave/real_overall.xlsx
@@ -508,7 +508,7 @@
         <v>0</v>
       </c>
       <c r="E2" t="n">
-        <v>61.4469051361084</v>
+        <v>61.91587448120117</v>
       </c>
       <c r="F2" t="n">
         <v>0</v>
@@ -532,7 +532,7 @@
         <v>0</v>
       </c>
       <c r="E3" t="n">
-        <v>114.3857836723328</v>
+        <v>113.3610486984253</v>
       </c>
       <c r="F3" t="n">
         <v>0.04516885553470926</v>
@@ -556,7 +556,7 @@
         <v>0</v>
       </c>
       <c r="E4" t="n">
-        <v>158.9834690093994</v>
+        <v>159.392237663269</v>
       </c>
       <c r="F4" t="n">
         <v>0.9736842105263158</v>
@@ -580,7 +580,7 @@
         <v>0</v>
       </c>
       <c r="E5" t="n">
-        <v>197.0813274383545</v>
+        <v>195.9049701690674</v>
       </c>
       <c r="F5" t="n">
         <v>1</v>
@@ -604,7 +604,7 @@
         <v>0</v>
       </c>
       <c r="E6" t="n">
-        <v>210.39217710495</v>
+        <v>208.9052796363831</v>
       </c>
       <c r="F6" t="n">
         <v>1</v>
@@ -628,7 +628,7 @@
         <v>0</v>
       </c>
       <c r="E7" t="n">
-        <v>229.6232342720032</v>
+        <v>228.295361995697</v>
       </c>
       <c r="F7" t="n">
         <v>1</v>
@@ -652,7 +652,7 @@
         <v>0</v>
       </c>
       <c r="E8" t="n">
-        <v>947360.002040863</v>
+        <v>865167.9310798645</v>
       </c>
       <c r="F8" t="n">
         <v>1</v>
@@ -728,7 +728,7 @@
         <v>0</v>
       </c>
       <c r="E11" t="n">
-        <v>47.71411418914795</v>
+        <v>47.99246788024902</v>
       </c>
       <c r="F11" t="n">
         <v>0.08522727272727272</v>
@@ -752,7 +752,7 @@
         <v>0</v>
       </c>
       <c r="E12" t="n">
-        <v>67.60001182556152</v>
+        <v>67.71337985992432</v>
       </c>
       <c r="F12" t="n">
         <v>0.5384615384615384</v>
@@ -776,7 +776,7 @@
         <v>0</v>
       </c>
       <c r="E13" t="n">
-        <v>84.39451456069946</v>
+        <v>83.60910415649414</v>
       </c>
       <c r="F13" t="n">
         <v>0.9266034327009938</v>
@@ -800,7 +800,7 @@
         <v>1</v>
       </c>
       <c r="E14" t="n">
-        <v>95.12854814529419</v>
+        <v>93.8071608543396</v>
       </c>
       <c r="F14" t="n">
         <v>0.9772727272727273</v>
@@ -824,7 +824,7 @@
         <v>1</v>
       </c>
       <c r="E15" t="n">
-        <v>1027272.235155106</v>
+        <v>293274.8041152954</v>
       </c>
       <c r="F15" t="n">
         <v>1</v>
@@ -852,7 +852,7 @@
         <v>0</v>
       </c>
       <c r="E16" t="n">
-        <v>10.55812835693359</v>
+        <v>10.19382476806641</v>
       </c>
       <c r="F16" t="n">
         <v>0</v>
@@ -876,7 +876,7 @@
         <v>0</v>
       </c>
       <c r="E17" t="n">
-        <v>14.80237245559692</v>
+        <v>14.39611911773682</v>
       </c>
       <c r="F17" t="n">
         <v>0</v>
@@ -900,7 +900,7 @@
         <v>0</v>
       </c>
       <c r="E18" t="n">
-        <v>18.50450038909912</v>
+        <v>18.35793256759644</v>
       </c>
       <c r="F18" t="n">
         <v>0.9773989898989899</v>
@@ -924,7 +924,7 @@
         <v>0</v>
       </c>
       <c r="E19" t="n">
-        <v>22.92704582214355</v>
+        <v>22.87697792053223</v>
       </c>
       <c r="F19" t="n">
         <v>1</v>
@@ -948,7 +948,7 @@
         <v>0</v>
       </c>
       <c r="E20" t="n">
-        <v>23.75596761703491</v>
+        <v>23.88185262680054</v>
       </c>
       <c r="F20" t="n">
         <v>1</v>
@@ -972,7 +972,7 @@
         <v>0</v>
       </c>
       <c r="E21" t="n">
-        <v>25.59356689453125</v>
+        <v>25.51437616348267</v>
       </c>
       <c r="F21" t="n">
         <v>1</v>
@@ -996,7 +996,7 @@
         <v>0</v>
       </c>
       <c r="E22" t="n">
-        <v>45.31693458557129</v>
+        <v>293192.8429603577</v>
       </c>
       <c r="F22" t="n">
         <v>1</v>
@@ -1024,7 +1024,7 @@
         <v>0</v>
       </c>
       <c r="E23" t="n">
-        <v>10.35380363464355</v>
+        <v>9.02104377746582</v>
       </c>
       <c r="F23" t="n">
         <v>0</v>
@@ -1048,7 +1048,7 @@
         <v>0</v>
       </c>
       <c r="E24" t="n">
-        <v>14.6068811416626</v>
+        <v>13.05216550827026</v>
       </c>
       <c r="F24" t="n">
         <v>0</v>
@@ -1066,19 +1066,19 @@
         <v>0.25</v>
       </c>
       <c r="C25" t="n">
-        <v>0.8980769230769231</v>
+        <v>0.8338607594936709</v>
       </c>
       <c r="D25" t="n">
         <v>0</v>
       </c>
       <c r="E25" t="n">
-        <v>18.28336715698242</v>
+        <v>16.32720232009888</v>
       </c>
       <c r="F25" t="n">
-        <v>0.9773989898989899</v>
+        <v>0.9738529014844804</v>
       </c>
       <c r="G25" t="n">
-        <v>0.8796791443850267</v>
+        <v>0.7848075348075347</v>
       </c>
       <c r="H25" t="n">
         <v>60</v>
@@ -1090,19 +1090,19 @@
         <v>0.5</v>
       </c>
       <c r="C26" t="n">
-        <v>0.9791666666666666</v>
+        <v>0.9705882352941176</v>
       </c>
       <c r="D26" t="n">
         <v>0</v>
       </c>
       <c r="E26" t="n">
-        <v>22.47047424316406</v>
+        <v>20.3709602355957</v>
       </c>
       <c r="F26" t="n">
         <v>1</v>
       </c>
       <c r="G26" t="n">
-        <v>0.9722222222222222</v>
+        <v>0.9629629629629629</v>
       </c>
       <c r="H26" t="n">
         <v>72.0096012801707</v>
@@ -1114,13 +1114,13 @@
         <v>0.75</v>
       </c>
       <c r="C27" t="n">
-        <v>1</v>
+        <v>0.9934640522875817</v>
       </c>
       <c r="D27" t="n">
         <v>0</v>
       </c>
       <c r="E27" t="n">
-        <v>23.33343029022217</v>
+        <v>21.12871408462524</v>
       </c>
       <c r="F27" t="n">
         <v>1</v>
@@ -1144,7 +1144,7 @@
         <v>0</v>
       </c>
       <c r="E28" t="n">
-        <v>25.12226104736328</v>
+        <v>22.62958288192749</v>
       </c>
       <c r="F28" t="n">
         <v>1</v>
@@ -1168,7 +1168,7 @@
         <v>0</v>
       </c>
       <c r="E29" t="n">
-        <v>954233.4611415863</v>
+        <v>995372.3289966583</v>
       </c>
       <c r="F29" t="n">
         <v>1</v>
@@ -1268,7 +1268,7 @@
         <v>0</v>
       </c>
       <c r="E33" t="n">
-        <v>1.989006996154785</v>
+        <v>1.961946487426758</v>
       </c>
       <c r="F33" t="n">
         <v>0.9074074074074074</v>
@@ -1292,7 +1292,7 @@
         <v>1</v>
       </c>
       <c r="E34" t="n">
-        <v>2.639949321746826</v>
+        <v>2.634048461914062</v>
       </c>
       <c r="F34" t="n">
         <v>1</v>
@@ -1316,7 +1316,7 @@
         <v>1</v>
       </c>
       <c r="E35" t="n">
-        <v>8.520698547363253</v>
+        <v>4.368138313293456</v>
       </c>
       <c r="F35" t="n">
         <v>1</v>
@@ -1340,7 +1340,7 @@
         <v>1</v>
       </c>
       <c r="E36" t="n">
-        <v>152.601957321167</v>
+        <v>90.25192260742188</v>
       </c>
       <c r="F36" t="n">
         <v>1</v>
@@ -1392,7 +1392,7 @@
         <v>0</v>
       </c>
       <c r="E38" t="n">
-        <v>60.72067022323608</v>
+        <v>60.20407676696777</v>
       </c>
       <c r="F38" t="n">
         <v>0.7145909090909092</v>
@@ -1416,7 +1416,7 @@
         <v>0</v>
       </c>
       <c r="E39" t="n">
-        <v>84.59854125976562</v>
+        <v>85.50363779067993</v>
       </c>
       <c r="F39" t="n">
         <v>0.972972972972973</v>
@@ -1440,7 +1440,7 @@
         <v>0</v>
       </c>
       <c r="E40" t="n">
-        <v>120.7020282745361</v>
+        <v>119.3625926971436</v>
       </c>
       <c r="F40" t="n">
         <v>1</v>
@@ -1464,7 +1464,7 @@
         <v>0</v>
       </c>
       <c r="E41" t="n">
-        <v>134.2943906784058</v>
+        <v>136.11900806427</v>
       </c>
       <c r="F41" t="n">
         <v>1</v>
@@ -1488,7 +1488,7 @@
         <v>0</v>
       </c>
       <c r="E42" t="n">
-        <v>142.3428535461426</v>
+        <v>145.0353503227234</v>
       </c>
       <c r="F42" t="n">
         <v>1</v>
@@ -1512,7 +1512,7 @@
         <v>1</v>
       </c>
       <c r="E43" t="n">
-        <v>158.9829921722412</v>
+        <v>212.2581005096436</v>
       </c>
       <c r="F43" t="n">
         <v>1</v>
@@ -1540,7 +1540,7 @@
         <v>0</v>
       </c>
       <c r="E44" t="n">
-        <v>5.333900451660156</v>
+        <v>4.981040954589844</v>
       </c>
       <c r="F44" t="n">
         <v>0</v>
@@ -1564,7 +1564,7 @@
         <v>0</v>
       </c>
       <c r="E45" t="n">
-        <v>8.173215389251709</v>
+        <v>7.868587970733643</v>
       </c>
       <c r="F45" t="n">
         <v>0</v>
@@ -1588,7 +1588,7 @@
         <v>0</v>
       </c>
       <c r="E46" t="n">
-        <v>10.96659898757935</v>
+        <v>10.69271564483643</v>
       </c>
       <c r="F46" t="n">
         <v>0.976328903654485</v>
@@ -1612,7 +1612,7 @@
         <v>0</v>
       </c>
       <c r="E47" t="n">
-        <v>16.76952838897705</v>
+        <v>16.26861095428467</v>
       </c>
       <c r="F47" t="n">
         <v>1</v>
@@ -1636,7 +1636,7 @@
         <v>0</v>
       </c>
       <c r="E48" t="n">
-        <v>19.13106441497803</v>
+        <v>18.64022016525269</v>
       </c>
       <c r="F48" t="n">
         <v>1</v>
@@ -1660,7 +1660,7 @@
         <v>0</v>
       </c>
       <c r="E49" t="n">
-        <v>21.23038768768311</v>
+        <v>20.59328556060791</v>
       </c>
       <c r="F49" t="n">
         <v>1</v>
@@ -1684,7 +1684,7 @@
         <v>0</v>
       </c>
       <c r="E50" t="n">
-        <v>27.92692184448242</v>
+        <v>40.16709327697754</v>
       </c>
       <c r="F50" t="n">
         <v>1</v>
@@ -1736,7 +1736,7 @@
         <v>0</v>
       </c>
       <c r="E52" t="n">
-        <v>1.476649997383356</v>
+        <v>1.489649998955429</v>
       </c>
       <c r="F52" t="n">
         <v>0.1</v>
@@ -1760,7 +1760,7 @@
         <v>0</v>
       </c>
       <c r="E53" t="n">
-        <v>2.523749999701977</v>
+        <v>2.518249998800457</v>
       </c>
       <c r="F53" t="n">
         <v>0.647456279809221</v>
@@ -1784,7 +1784,7 @@
         <v>0</v>
       </c>
       <c r="E54" t="n">
-        <v>2.911499999463558</v>
+        <v>2.885500002652407</v>
       </c>
       <c r="F54" t="n">
         <v>0.9375</v>
@@ -1808,7 +1808,7 @@
         <v>0</v>
       </c>
       <c r="E55" t="n">
-        <v>3.124749999493361</v>
+        <v>3.099999996833503</v>
       </c>
       <c r="F55" t="n">
         <v>1</v>
@@ -1832,7 +1832,7 @@
         <v>0</v>
       </c>
       <c r="E56" t="n">
-        <v>3.637249999493359</v>
+        <v>3.544799996167421</v>
       </c>
       <c r="F56" t="n">
         <v>1</v>
@@ -1856,7 +1856,7 @@
         <v>1</v>
       </c>
       <c r="E57" t="n">
-        <v>53.7339999973774</v>
+        <v>94.54900000244379</v>
       </c>
       <c r="F57" t="n">
         <v>1</v>
@@ -1884,7 +1884,7 @@
         <v>0</v>
       </c>
       <c r="E58" t="n">
-        <v>1.675128936767578</v>
+        <v>1.650094985961914</v>
       </c>
       <c r="F58" t="n">
         <v>0</v>
@@ -1908,7 +1908,7 @@
         <v>0</v>
       </c>
       <c r="E59" t="n">
-        <v>1.883184909820557</v>
+        <v>1.862752437591553</v>
       </c>
       <c r="F59" t="n">
         <v>0</v>
@@ -1932,7 +1932,7 @@
         <v>0</v>
       </c>
       <c r="E60" t="n">
-        <v>1.99204683303833</v>
+        <v>1.988232135772705</v>
       </c>
       <c r="F60" t="n">
         <v>0.8636363636363636</v>
@@ -1956,7 +1956,7 @@
         <v>0</v>
       </c>
       <c r="E61" t="n">
-        <v>2.162933349609375</v>
+        <v>2.152919769287109</v>
       </c>
       <c r="F61" t="n">
         <v>0.9767441860465116</v>
@@ -1980,7 +1980,7 @@
         <v>0</v>
       </c>
       <c r="E62" t="n">
-        <v>2.250909805297852</v>
+        <v>2.233207225799561</v>
       </c>
       <c r="F62" t="n">
         <v>1</v>
@@ -2004,7 +2004,7 @@
         <v>0</v>
       </c>
       <c r="E63" t="n">
-        <v>2.416729927062988</v>
+        <v>2.337312698364258</v>
       </c>
       <c r="F63" t="n">
         <v>1</v>
@@ -2028,7 +2028,7 @@
         <v>0</v>
       </c>
       <c r="E64" t="n">
-        <v>14.11795616149902</v>
+        <v>60.42885780334473</v>
       </c>
       <c r="F64" t="n">
         <v>1</v>
@@ -2056,7 +2056,7 @@
         <v>0</v>
       </c>
       <c r="E65" t="n">
-        <v>1.711130142211914</v>
+        <v>1.717090606689453</v>
       </c>
       <c r="F65" t="n">
         <v>0</v>
@@ -2080,7 +2080,7 @@
         <v>0</v>
       </c>
       <c r="E66" t="n">
-        <v>2.336025238037109</v>
+        <v>2.348566055297852</v>
       </c>
       <c r="F66" t="n">
         <v>0</v>
@@ -2104,7 +2104,7 @@
         <v>0</v>
       </c>
       <c r="E67" t="n">
-        <v>2.689719200134277</v>
+        <v>2.612411975860596</v>
       </c>
       <c r="F67" t="n">
         <v>0</v>
@@ -2128,7 +2128,7 @@
         <v>0</v>
       </c>
       <c r="E68" t="n">
-        <v>3.258943557739258</v>
+        <v>3.137588500976562</v>
       </c>
       <c r="F68" t="n">
         <v>0.1762749445676275</v>
@@ -2152,7 +2152,7 @@
         <v>0</v>
       </c>
       <c r="E69" t="n">
-        <v>3.730952739715576</v>
+        <v>3.612220287322998</v>
       </c>
       <c r="F69" t="n">
         <v>0.9776515151515152</v>
@@ -2176,7 +2176,7 @@
         <v>0</v>
       </c>
       <c r="E70" t="n">
-        <v>4.696130752563477</v>
+        <v>4.477226734161376</v>
       </c>
       <c r="F70" t="n">
         <v>1</v>
@@ -2200,7 +2200,7 @@
         <v>0</v>
       </c>
       <c r="E71" t="n">
-        <v>22.63689041137695</v>
+        <v>22.4609375</v>
       </c>
       <c r="F71" t="n">
         <v>1</v>
@@ -2228,7 +2228,7 @@
         <v>0</v>
       </c>
       <c r="E72" t="n">
-        <v>7.056951522827148</v>
+        <v>6.799221038818359</v>
       </c>
       <c r="F72" t="n">
         <v>0</v>
@@ -2252,7 +2252,7 @@
         <v>0</v>
       </c>
       <c r="E73" t="n">
-        <v>12.92506456375122</v>
+        <v>12.29087114334106</v>
       </c>
       <c r="F73" t="n">
         <v>0.3564849624060151</v>
@@ -2276,7 +2276,7 @@
         <v>0</v>
       </c>
       <c r="E74" t="n">
-        <v>18.4590220451355</v>
+        <v>17.89242029190063</v>
       </c>
       <c r="F74" t="n">
         <v>0.7272727272727273</v>
@@ -2300,7 +2300,7 @@
         <v>0</v>
       </c>
       <c r="E75" t="n">
-        <v>25.61104297637939</v>
+        <v>25.15101432800293</v>
       </c>
       <c r="F75" t="n">
         <v>0.925</v>
@@ -2324,7 +2324,7 @@
         <v>0</v>
       </c>
       <c r="E76" t="n">
-        <v>26.13800764083862</v>
+        <v>25.39414167404175</v>
       </c>
       <c r="F76" t="n">
         <v>0.9714285714285714</v>
@@ -2348,7 +2348,7 @@
         <v>0</v>
       </c>
       <c r="E77" t="n">
-        <v>26.99217796325684</v>
+        <v>25.90879201889038</v>
       </c>
       <c r="F77" t="n">
         <v>1</v>
@@ -2372,7 +2372,7 @@
         <v>0</v>
       </c>
       <c r="E78" t="n">
-        <v>36.86189651489258</v>
+        <v>30.94387054443359</v>
       </c>
       <c r="F78" t="n">
         <v>1</v>
@@ -2400,7 +2400,7 @@
         <v>0</v>
       </c>
       <c r="E79" t="n">
-        <v>2.114057540893555</v>
+        <v>2.050161361694336</v>
       </c>
       <c r="F79" t="n">
         <v>0</v>
@@ -2424,7 +2424,7 @@
         <v>0</v>
       </c>
       <c r="E80" t="n">
-        <v>2.289128303527832</v>
+        <v>2.219116687774658</v>
       </c>
       <c r="F80" t="n">
         <v>0.7676470588235295</v>
@@ -2448,7 +2448,7 @@
         <v>0</v>
       </c>
       <c r="E81" t="n">
-        <v>2.493202686309814</v>
+        <v>2.424299716949463</v>
       </c>
       <c r="F81" t="n">
         <v>0.9710144927536232</v>
@@ -2472,7 +2472,7 @@
         <v>0</v>
       </c>
       <c r="E82" t="n">
-        <v>2.645015716552734</v>
+        <v>2.60007381439209</v>
       </c>
       <c r="F82" t="n">
         <v>1</v>
@@ -2496,7 +2496,7 @@
         <v>0</v>
       </c>
       <c r="E83" t="n">
-        <v>2.791881561279297</v>
+        <v>2.744913101196289</v>
       </c>
       <c r="F83" t="n">
         <v>1</v>
@@ -2520,7 +2520,7 @@
         <v>0</v>
       </c>
       <c r="E84" t="n">
-        <v>3.128969669342041</v>
+        <v>3.067731857299804</v>
       </c>
       <c r="F84" t="n">
         <v>1</v>
@@ -2544,7 +2544,7 @@
         <v>0</v>
       </c>
       <c r="E85" t="n">
-        <v>3.875970840454102</v>
+        <v>8.311033248901367</v>
       </c>
       <c r="F85" t="n">
         <v>1</v>
@@ -2572,7 +2572,7 @@
         <v>0</v>
       </c>
       <c r="E86" t="n">
-        <v>1.2359619140625</v>
+        <v>1.193046569824219</v>
       </c>
       <c r="F86" t="n">
         <v>0</v>
@@ -2596,7 +2596,7 @@
         <v>0</v>
       </c>
       <c r="E87" t="n">
-        <v>1.332998275756836</v>
+        <v>1.302719116210938</v>
       </c>
       <c r="F87" t="n">
         <v>0</v>
@@ -2620,7 +2620,7 @@
         <v>0</v>
       </c>
       <c r="E88" t="n">
-        <v>1.651287078857422</v>
+        <v>1.600265502929688</v>
       </c>
       <c r="F88" t="n">
         <v>0.9781249999999999</v>
@@ -2644,7 +2644,7 @@
         <v>0</v>
       </c>
       <c r="E89" t="n">
-        <v>2.035021781921387</v>
+        <v>2.04002857208252</v>
       </c>
       <c r="F89" t="n">
         <v>1</v>
@@ -2668,7 +2668,7 @@
         <v>0</v>
       </c>
       <c r="E90" t="n">
-        <v>2.283036708831787</v>
+        <v>2.304792404174805</v>
       </c>
       <c r="F90" t="n">
         <v>1</v>
@@ -2692,7 +2692,7 @@
         <v>0</v>
       </c>
       <c r="E91" t="n">
-        <v>2.688336372375487</v>
+        <v>2.665376663208008</v>
       </c>
       <c r="F91" t="n">
         <v>1</v>
@@ -2716,7 +2716,7 @@
         <v>0</v>
       </c>
       <c r="E92" t="n">
-        <v>5.067110061645508</v>
+        <v>9.670734405517578</v>
       </c>
       <c r="F92" t="n">
         <v>1</v>
@@ -2768,7 +2768,7 @@
         <v>0</v>
       </c>
       <c r="E94" t="n">
-        <v>1.753849998116493</v>
+        <v>1.716300001367927</v>
       </c>
       <c r="F94" t="n">
         <v>0.5</v>
@@ -2792,7 +2792,7 @@
         <v>0</v>
       </c>
       <c r="E95" t="n">
-        <v>2.103999990038574</v>
+        <v>2.034250000491738</v>
       </c>
       <c r="F95" t="n">
         <v>0.9565217391304348</v>
@@ -2816,7 +2816,7 @@
         <v>0</v>
       </c>
       <c r="E96" t="n">
-        <v>2.310000002384186</v>
+        <v>2.268499996513128</v>
       </c>
       <c r="F96" t="n">
         <v>1</v>
@@ -2840,7 +2840,7 @@
         <v>0</v>
       </c>
       <c r="E97" t="n">
-        <v>2.718499997630715</v>
+        <v>2.668499996885657</v>
       </c>
       <c r="F97" t="n">
         <v>1</v>
@@ -2864,7 +2864,7 @@
         <v>0</v>
       </c>
       <c r="E98" t="n">
-        <v>4.760399999842047</v>
+        <v>4.646150003001093</v>
       </c>
       <c r="F98" t="n">
         <v>1</v>
@@ -2888,7 +2888,7 @@
         <v>1</v>
       </c>
       <c r="E99" t="n">
-        <v>30.26700000092387</v>
+        <v>32.17499999701977</v>
       </c>
       <c r="F99" t="n">
         <v>1</v>
@@ -2940,7 +2940,7 @@
         <v>0</v>
       </c>
       <c r="E101" t="n">
-        <v>0.6206500012427568</v>
+        <v>0.6296499971300363</v>
       </c>
       <c r="F101" t="n">
         <v>0</v>
@@ -2964,7 +2964,7 @@
         <v>0</v>
       </c>
       <c r="E102" t="n">
-        <v>0.8149999981978908</v>
+        <v>0.8002500031143427</v>
       </c>
       <c r="F102" t="n">
         <v>0.945933014354067</v>
@@ -2988,7 +2988,7 @@
         <v>0</v>
       </c>
       <c r="E103" t="n">
-        <v>0.9660000037401915</v>
+        <v>0.96000000461936</v>
       </c>
       <c r="F103" t="n">
         <v>1</v>
@@ -3012,7 +3012,7 @@
         <v>0</v>
       </c>
       <c r="E104" t="n">
-        <v>1.35050000436604</v>
+        <v>1.33124999050051</v>
       </c>
       <c r="F104" t="n">
         <v>1</v>
@@ -3036,7 +3036,7 @@
         <v>0</v>
       </c>
       <c r="E105" t="n">
-        <v>1.841750001907348</v>
+        <v>1.815750003606081</v>
       </c>
       <c r="F105" t="n">
         <v>1</v>
@@ -3060,7 +3060,7 @@
         <v>1</v>
       </c>
       <c r="E106" t="n">
-        <v>8.802999999374151</v>
+        <v>9.525999993085861</v>
       </c>
       <c r="F106" t="n">
         <v>1</v>
@@ -3088,7 +3088,7 @@
         <v>0</v>
       </c>
       <c r="E107" t="n">
-        <v>2.819061279296875</v>
+        <v>2.655982971191406</v>
       </c>
       <c r="F107" t="n">
         <v>0</v>
@@ -3112,7 +3112,7 @@
         <v>0</v>
       </c>
       <c r="E108" t="n">
-        <v>5.181944370269775</v>
+        <v>4.889726638793945</v>
       </c>
       <c r="F108" t="n">
         <v>0.9230769230769231</v>
@@ -3136,7 +3136,7 @@
         <v>0</v>
       </c>
       <c r="E109" t="n">
-        <v>6.720185279846191</v>
+        <v>6.480157375335693</v>
       </c>
       <c r="F109" t="n">
         <v>0.9757549361207898</v>
@@ -3160,7 +3160,7 @@
         <v>0</v>
       </c>
       <c r="E110" t="n">
-        <v>9.031414985656738</v>
+        <v>8.646011352539062</v>
       </c>
       <c r="F110" t="n">
         <v>1</v>
@@ -3184,7 +3184,7 @@
         <v>0</v>
       </c>
       <c r="E111" t="n">
-        <v>9.209811687469482</v>
+        <v>8.827269077301025</v>
       </c>
       <c r="F111" t="n">
         <v>1</v>
@@ -3208,7 +3208,7 @@
         <v>0</v>
       </c>
       <c r="E112" t="n">
-        <v>9.521198272705076</v>
+        <v>8.926045894622803</v>
       </c>
       <c r="F112" t="n">
         <v>1</v>
@@ -3232,7 +3232,7 @@
         <v>0</v>
       </c>
       <c r="E113" t="n">
-        <v>9.8419189453125</v>
+        <v>13.62109184265137</v>
       </c>
       <c r="F113" t="n">
         <v>1</v>
@@ -3260,7 +3260,7 @@
         <v>0</v>
       </c>
       <c r="E114" t="n">
-        <v>8.315999999642372</v>
+        <v>8.629000000655651</v>
       </c>
       <c r="F114" t="n">
         <v>0</v>
@@ -3284,7 +3284,7 @@
         <v>0</v>
       </c>
       <c r="E115" t="n">
-        <v>12.2229499951005</v>
+        <v>12.3289999961853</v>
       </c>
       <c r="F115" t="n">
         <v>0.8991025641025642</v>
@@ -3308,7 +3308,7 @@
         <v>0</v>
       </c>
       <c r="E116" t="n">
-        <v>18.21375000290573</v>
+        <v>17.54925000108778</v>
       </c>
       <c r="F116" t="n">
         <v>1</v>
@@ -3332,7 +3332,7 @@
         <v>0</v>
       </c>
       <c r="E117" t="n">
-        <v>37.83449999988079</v>
+        <v>36.60999999940395</v>
       </c>
       <c r="F117" t="n">
         <v>1</v>
@@ -3356,7 +3356,7 @@
         <v>0</v>
       </c>
       <c r="E118" t="n">
-        <v>40.69000000320375</v>
+        <v>39.41549999639392</v>
       </c>
       <c r="F118" t="n">
         <v>1</v>
@@ -3380,7 +3380,7 @@
         <v>0</v>
       </c>
       <c r="E119" t="n">
-        <v>48.10405000336468</v>
+        <v>45.6207500046119</v>
       </c>
       <c r="F119" t="n">
         <v>1</v>
@@ -3404,7 +3404,7 @@
         <v>0</v>
       </c>
       <c r="E120" t="n">
-        <v>106.1840000003576</v>
+        <v>154.875</v>
       </c>
       <c r="F120" t="n">
         <v>1</v>
@@ -3432,7 +3432,7 @@
         <v>0</v>
       </c>
       <c r="E121" t="n">
-        <v>64.55612182617188</v>
+        <v>63.06099891662598</v>
       </c>
       <c r="F121" t="n">
         <v>0</v>
@@ -3456,7 +3456,7 @@
         <v>0</v>
       </c>
       <c r="E122" t="n">
-        <v>129.6574711799622</v>
+        <v>126.7129898071289</v>
       </c>
       <c r="F122" t="n">
         <v>0.6</v>
@@ -3480,7 +3480,7 @@
         <v>0</v>
       </c>
       <c r="E123" t="n">
-        <v>184.79984998703</v>
+        <v>182.6382875442505</v>
       </c>
       <c r="F123" t="n">
         <v>0.8521241830065359</v>
@@ -3504,7 +3504,7 @@
         <v>0</v>
       </c>
       <c r="E124" t="n">
-        <v>256.0614347457886</v>
+        <v>253.0834674835205</v>
       </c>
       <c r="F124" t="n">
         <v>1</v>
@@ -3528,7 +3528,7 @@
         <v>0</v>
       </c>
       <c r="E125" t="n">
-        <v>259.9309682846069</v>
+        <v>254.905104637146</v>
       </c>
       <c r="F125" t="n">
         <v>1</v>
@@ -3552,7 +3552,7 @@
         <v>0</v>
       </c>
       <c r="E126" t="n">
-        <v>266.3999915122986</v>
+        <v>259.7604274749756</v>
       </c>
       <c r="F126" t="n">
         <v>1</v>
@@ -3576,7 +3576,7 @@
         <v>0</v>
       </c>
       <c r="E127" t="n">
-        <v>955452.7499675751</v>
+        <v>293460.0381851196</v>
       </c>
       <c r="F127" t="n">
         <v>1</v>

</xml_diff>